<commit_message>
Added pie chart graph for community data to app.
</commit_message>
<xml_diff>
--- a/Data/new_crosswalk.xlsx
+++ b/Data/new_crosswalk.xlsx
@@ -15,7 +15,7 @@
     <sheet name="LCD" sheetId="4" r:id="rId1"/>
     <sheet name="Hierarchy2" sheetId="6" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1783" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1838" uniqueCount="500">
   <si>
     <t>ACARTELA</t>
   </si>
@@ -737,9 +737,6 @@
     <t>Juvenile</t>
   </si>
   <si>
-    <t>All</t>
-  </si>
-  <si>
     <t>Larvae</t>
   </si>
   <si>
@@ -1253,9 +1250,6 @@
     <t>twentymmstart2</t>
   </si>
   <si>
-    <t>Yolo</t>
-  </si>
-  <si>
     <t>Acanthocyclops vernalis NA</t>
   </si>
   <si>
@@ -1608,6 +1602,12 @@
   </si>
   <si>
     <t>Oithona spp_</t>
+  </si>
+  <si>
+    <t>YBFMP</t>
+  </si>
+  <si>
+    <t>Mixed</t>
   </si>
 </sst>
 </file>
@@ -1947,7 +1947,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2107,10 +2107,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
@@ -3300,8 +3296,8 @@
   <dimension ref="A1:V171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3341,13 +3337,13 @@
         <v>205</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E1" s="66" t="s">
-        <v>381</v>
+        <v>498</v>
       </c>
       <c r="F1" s="58" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G1" s="22" t="s">
         <v>204</v>
@@ -3374,28 +3370,28 @@
         <v>87</v>
       </c>
       <c r="O1" s="78" t="s">
+        <v>372</v>
+      </c>
+      <c r="P1" s="79" t="s">
         <v>373</v>
       </c>
-      <c r="P1" s="79" t="s">
+      <c r="Q1" s="78" t="s">
         <v>374</v>
       </c>
-      <c r="Q1" s="78" t="s">
+      <c r="R1" s="78" t="s">
         <v>375</v>
       </c>
-      <c r="R1" s="78" t="s">
+      <c r="S1" s="78" t="s">
         <v>376</v>
       </c>
-      <c r="S1" s="78" t="s">
+      <c r="T1" s="78" t="s">
         <v>377</v>
       </c>
-      <c r="T1" s="78" t="s">
+      <c r="U1" s="78" t="s">
         <v>378</v>
       </c>
-      <c r="U1" s="78" t="s">
+      <c r="V1" s="78" t="s">
         <v>379</v>
-      </c>
-      <c r="V1" s="78" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3412,7 +3408,7 @@
         <v>119</v>
       </c>
       <c r="E2" s="85" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F2" s="58" t="s">
         <v>207</v>
@@ -3462,7 +3458,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D3" s="69"/>
       <c r="E3" s="69"/>
@@ -3505,7 +3501,7 @@
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
       <c r="C4" s="7" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D4" s="69"/>
       <c r="E4" s="69"/>
@@ -3546,7 +3542,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="68" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E5" s="85"/>
       <c r="F5" s="58" t="s">
@@ -3587,13 +3583,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D6" s="68" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="85" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F6" s="58" t="s">
         <v>207</v>
@@ -3642,7 +3638,7 @@
         <v>118</v>
       </c>
       <c r="E7" s="85" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F7" s="58" t="s">
         <v>207</v>
@@ -3683,7 +3679,7 @@
       </c>
       <c r="D8" s="69"/>
       <c r="E8" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F8" s="58" t="s">
         <v>207</v>
@@ -3721,10 +3717,10 @@
         <v>130</v>
       </c>
       <c r="D9" s="68" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E9" s="85" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F9" s="58" t="s">
         <v>207</v>
@@ -3761,7 +3757,7 @@
       <c r="A10" s="32"/>
       <c r="B10" s="33"/>
       <c r="C10" s="34" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D10" s="69"/>
       <c r="E10" s="69"/>
@@ -3811,7 +3807,7 @@
         <v>10</v>
       </c>
       <c r="E11" s="85" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F11" s="58" t="s">
         <v>207</v>
@@ -3956,7 +3952,7 @@
         <v>117</v>
       </c>
       <c r="E14" s="85" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F14" s="58" t="s">
         <v>207</v>
@@ -4004,17 +4000,35 @@
       <c r="C15" s="7"/>
       <c r="D15" s="68"/>
       <c r="E15" s="85" t="s">
-        <v>409</v>
-      </c>
-      <c r="F15" s="58"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="45"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="39"/>
+        <v>407</v>
+      </c>
+      <c r="F15" s="58" t="s">
+        <v>207</v>
+      </c>
+      <c r="G15" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="I15" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="J15" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="K15" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="L15" s="45" t="s">
+        <v>191</v>
+      </c>
+      <c r="M15" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="N15" s="39" t="s">
+        <v>14</v>
+      </c>
       <c r="O15" s="80"/>
     </row>
     <row r="16" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4164,7 +4178,7 @@
         <v>105</v>
       </c>
       <c r="E19" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="F19" s="58" t="s">
         <v>207</v>
@@ -4215,17 +4229,35 @@
       <c r="C20" s="7"/>
       <c r="D20" s="68"/>
       <c r="E20" t="s">
-        <v>408</v>
-      </c>
-      <c r="F20" s="58"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="87"/>
+        <v>406</v>
+      </c>
+      <c r="F20" s="58" t="s">
+        <v>207</v>
+      </c>
+      <c r="G20" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="J20" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="K20" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="L20" s="47" t="s">
+        <v>193</v>
+      </c>
+      <c r="M20" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="N20" s="39" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="21" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
@@ -4235,7 +4267,7 @@
         <v>18</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D21" s="68" t="s">
         <v>80</v>
@@ -4245,7 +4277,7 @@
         <v>207</v>
       </c>
       <c r="G21" s="49" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H21" s="48" t="s">
         <v>86</v>
@@ -4263,7 +4295,7 @@
         <v>194</v>
       </c>
       <c r="M21" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N21" s="37"/>
       <c r="O21" s="80">
@@ -4310,7 +4342,7 @@
         <v>194</v>
       </c>
       <c r="M22" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N22" s="49" t="s">
         <v>20</v>
@@ -4340,7 +4372,7 @@
       </c>
       <c r="D23" s="69"/>
       <c r="E23" s="69" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F23" s="58" t="s">
         <v>207</v>
@@ -4364,7 +4396,7 @@
         <v>194</v>
       </c>
       <c r="M23" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N23" s="49" t="s">
         <v>22</v>
@@ -4488,7 +4520,7 @@
         <v>70</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D26" s="68" t="s">
         <v>81</v>
@@ -4532,10 +4564,10 @@
         <v>107</v>
       </c>
       <c r="D27" s="68" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E27" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F27" s="58" t="s">
         <v>207</v>
@@ -4571,7 +4603,7 @@
       </c>
       <c r="D28" s="69"/>
       <c r="E28" s="69" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F28" s="58" t="s">
         <v>207</v>
@@ -4618,10 +4650,10 @@
         <v>132</v>
       </c>
       <c r="E29" s="85" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F29" s="58" t="s">
-        <v>209</v>
+        <v>499</v>
       </c>
       <c r="G29" s="37" t="s">
         <v>133</v>
@@ -4656,10 +4688,10 @@
         <v>71</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D30" s="68" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E30" s="85"/>
       <c r="F30" s="58" t="s">
@@ -4707,7 +4739,7 @@
         <v>122</v>
       </c>
       <c r="E31" s="85" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F31" s="58" t="s">
         <v>208</v>
@@ -4755,7 +4787,7 @@
       </c>
       <c r="D32" s="69"/>
       <c r="E32" s="69" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F32" s="58" t="s">
         <v>208</v>
@@ -5162,10 +5194,10 @@
         <v>103</v>
       </c>
       <c r="D41" s="68" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E41" s="85" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F41" s="58" t="s">
         <v>208</v>
@@ -5214,7 +5246,7 @@
         <v>208</v>
       </c>
       <c r="G42" s="39" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H42" s="40" t="s">
         <v>86</v>
@@ -5232,7 +5264,7 @@
         <v>194</v>
       </c>
       <c r="M42" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N42" s="37"/>
       <c r="O42" s="80">
@@ -5338,17 +5370,35 @@
       <c r="B45" s="10"/>
       <c r="D45" s="69"/>
       <c r="E45" t="s">
-        <v>410</v>
-      </c>
-      <c r="F45" s="58"/>
-      <c r="G45" s="49"/>
-      <c r="H45" s="48"/>
-      <c r="I45" s="37"/>
-      <c r="J45" s="37"/>
-      <c r="K45" s="88"/>
-      <c r="L45" s="60"/>
-      <c r="M45" s="60"/>
-      <c r="N45" s="42"/>
+        <v>408</v>
+      </c>
+      <c r="F45" s="58" t="s">
+        <v>208</v>
+      </c>
+      <c r="G45" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H45" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="I45" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="J45" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="K45" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="L45" s="47" t="s">
+        <v>193</v>
+      </c>
+      <c r="M45" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="N45" s="39" t="s">
+        <v>17</v>
+      </c>
       <c r="O45" s="80"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
@@ -5356,17 +5406,35 @@
       <c r="B46" s="10"/>
       <c r="D46" s="69"/>
       <c r="E46" s="74" t="s">
-        <v>402</v>
-      </c>
-      <c r="F46" s="58"/>
-      <c r="G46" s="49"/>
-      <c r="H46" s="48"/>
-      <c r="I46" s="37"/>
-      <c r="J46" s="37"/>
-      <c r="K46" s="88"/>
-      <c r="L46" s="60"/>
-      <c r="M46" s="60"/>
-      <c r="N46" s="42"/>
+        <v>400</v>
+      </c>
+      <c r="F46" s="58" t="s">
+        <v>208</v>
+      </c>
+      <c r="G46" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="I46" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="J46" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="K46" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="L46" s="45" t="s">
+        <v>191</v>
+      </c>
+      <c r="M46" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="N46" s="49" t="s">
+        <v>14</v>
+      </c>
       <c r="O46" s="80"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
@@ -5374,17 +5442,35 @@
       <c r="B47" s="10"/>
       <c r="D47" s="69"/>
       <c r="E47" t="s">
-        <v>411</v>
-      </c>
-      <c r="F47" s="58"/>
-      <c r="G47" s="49"/>
-      <c r="H47" s="48"/>
-      <c r="I47" s="37"/>
-      <c r="J47" s="37"/>
-      <c r="K47" s="88"/>
-      <c r="L47" s="60"/>
-      <c r="M47" s="60"/>
-      <c r="N47" s="42"/>
+        <v>409</v>
+      </c>
+      <c r="F47" s="58" t="s">
+        <v>208</v>
+      </c>
+      <c r="G47" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="H47" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="I47" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="J47" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="K47" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="L47" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="M47" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="N47" s="39" t="s">
+        <v>10</v>
+      </c>
       <c r="O47" s="80"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
@@ -5396,10 +5482,10 @@
       </c>
       <c r="D48" s="69"/>
       <c r="E48" s="69" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F48" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G48" s="49" t="s">
         <v>101</v>
@@ -5437,7 +5523,7 @@
       </c>
       <c r="E49" s="85"/>
       <c r="F49" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G49" s="44" t="s">
         <v>116</v>
@@ -5475,7 +5561,7 @@
       <c r="D50" s="69"/>
       <c r="E50" s="69"/>
       <c r="F50" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G50" s="49" t="s">
         <v>6</v>
@@ -5516,11 +5602,11 @@
         <v>45</v>
       </c>
       <c r="D51" s="68" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E51" s="85"/>
       <c r="F51" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G51" s="49" t="s">
         <v>101</v>
@@ -5560,7 +5646,7 @@
       </c>
       <c r="E52" s="85"/>
       <c r="F52" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G52" s="49" t="s">
         <v>114</v>
@@ -5606,7 +5692,7 @@
       <c r="D53" s="69"/>
       <c r="E53" s="69"/>
       <c r="F53" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G53" s="44" t="s">
         <v>117</v>
@@ -5649,7 +5735,7 @@
       </c>
       <c r="E54" s="85"/>
       <c r="F54" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G54" s="49" t="s">
         <v>14</v>
@@ -5690,12 +5776,20 @@
       <c r="B55" s="10"/>
       <c r="D55" s="68"/>
       <c r="E55" t="s">
-        <v>412</v>
-      </c>
-      <c r="F55" s="58"/>
-      <c r="G55" s="49"/>
-      <c r="H55" s="48"/>
-      <c r="I55" s="41"/>
+        <v>410</v>
+      </c>
+      <c r="F55" s="58" t="s">
+        <v>209</v>
+      </c>
+      <c r="G55" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="H55" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="I55" s="37" t="s">
+        <v>93</v>
+      </c>
       <c r="J55" s="41"/>
       <c r="K55" s="46"/>
       <c r="L55" s="45"/>
@@ -5708,14 +5802,26 @@
       <c r="B56" s="10"/>
       <c r="D56" s="68"/>
       <c r="E56" t="s">
-        <v>413</v>
-      </c>
-      <c r="F56" s="58"/>
-      <c r="G56" s="49"/>
-      <c r="H56" s="48"/>
-      <c r="I56" s="41"/>
-      <c r="J56" s="41"/>
-      <c r="K56" s="46"/>
+        <v>411</v>
+      </c>
+      <c r="F56" s="58" t="s">
+        <v>209</v>
+      </c>
+      <c r="G56" s="49" t="s">
+        <v>136</v>
+      </c>
+      <c r="H56" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="I56" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="J56" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="K56" s="46" t="s">
+        <v>136</v>
+      </c>
       <c r="L56" s="45"/>
       <c r="M56" s="42"/>
       <c r="N56" s="49"/>
@@ -5735,7 +5841,7 @@
         <v>134</v>
       </c>
       <c r="E57" s="85" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F57" s="58" t="s">
         <v>207</v>
@@ -5924,7 +6030,7 @@
         <v>136</v>
       </c>
       <c r="E61" s="85" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F61" s="58" t="s">
         <v>207</v>
@@ -6021,7 +6127,7 @@
         <v>91</v>
       </c>
       <c r="J63" s="37" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K63" s="37" t="s">
         <v>98</v>
@@ -6067,7 +6173,7 @@
         <v>91</v>
       </c>
       <c r="J64" s="37" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K64" s="37" t="s">
         <v>98</v>
@@ -6123,10 +6229,10 @@
         <v>90</v>
       </c>
       <c r="D66" s="68" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E66" s="85" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F66" s="58" t="s">
         <v>207</v>
@@ -6182,7 +6288,7 @@
         <v>91</v>
       </c>
       <c r="J67" s="37" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K67" s="37" t="s">
         <v>98</v>
@@ -6219,7 +6325,7 @@
         <v>207</v>
       </c>
       <c r="G68" s="49" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H68" s="48" t="s">
         <v>86</v>
@@ -6228,7 +6334,7 @@
         <v>91</v>
       </c>
       <c r="J68" s="37" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K68" s="37" t="s">
         <v>98</v>
@@ -6269,7 +6375,7 @@
         <v>91</v>
       </c>
       <c r="J69" s="37" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K69" s="37" t="s">
         <v>98</v>
@@ -6313,7 +6419,7 @@
         <v>91</v>
       </c>
       <c r="J70" s="37" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K70" s="37" t="s">
         <v>98</v>
@@ -6343,25 +6449,25 @@
         <v>99</v>
       </c>
       <c r="D71" s="68" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E71" s="85" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F71" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G71" s="46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H71" s="48" t="s">
         <v>188</v>
       </c>
       <c r="I71" s="41" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J71" s="46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K71" s="60"/>
       <c r="L71" s="60"/>
@@ -6390,7 +6496,7 @@
       <c r="D72" s="69"/>
       <c r="E72" s="69"/>
       <c r="F72" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G72" s="37" t="s">
         <v>144</v>
@@ -6422,7 +6528,7 @@
     </row>
     <row r="73" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="61" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>67</v>
@@ -6431,13 +6537,13 @@
         <v>67</v>
       </c>
       <c r="E73" s="85" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F73" s="58" t="s">
         <v>207</v>
       </c>
       <c r="G73" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H73" s="43" t="s">
         <v>83</v>
@@ -6446,7 +6552,7 @@
         <v>93</v>
       </c>
       <c r="J73" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K73" s="60"/>
       <c r="L73" s="60"/>
@@ -6509,7 +6615,7 @@
       </c>
       <c r="D75" s="70"/>
       <c r="E75" s="70" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F75" s="58" t="s">
         <v>207</v>
@@ -6542,13 +6648,13 @@
         <v>92</v>
       </c>
       <c r="D76" s="71" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E76" s="86" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F76" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G76" s="54" t="s">
         <v>95</v>
@@ -6584,13 +6690,13 @@
         <v>96</v>
       </c>
       <c r="D77" s="71" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E77" s="86" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F77" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G77" s="54" t="s">
         <v>94</v>
@@ -6617,7 +6723,7 @@
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C78" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D78" s="69"/>
       <c r="E78" s="69"/>
@@ -6625,7 +6731,7 @@
         <v>207</v>
       </c>
       <c r="G78" s="57" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H78" s="56" t="s">
         <v>87</v>
@@ -6637,16 +6743,16 @@
         <v>102</v>
       </c>
       <c r="K78" s="55" t="s">
+        <v>220</v>
+      </c>
+      <c r="L78" s="55" t="s">
         <v>221</v>
       </c>
-      <c r="L78" s="55" t="s">
+      <c r="M78" s="64" t="s">
         <v>222</v>
       </c>
-      <c r="M78" s="64" t="s">
-        <v>223</v>
-      </c>
       <c r="N78" s="57" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="O78" s="81">
         <v>1992</v>
@@ -6654,7 +6760,7 @@
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C79" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D79" s="69"/>
       <c r="E79" s="69"/>
@@ -6662,7 +6768,7 @@
         <v>207</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H79" s="65" t="s">
         <v>86</v>
@@ -6674,13 +6780,13 @@
         <v>102</v>
       </c>
       <c r="K79" s="64" t="s">
+        <v>224</v>
+      </c>
+      <c r="L79" s="64" t="s">
         <v>225</v>
       </c>
-      <c r="L79" s="64" t="s">
-        <v>226</v>
-      </c>
       <c r="M79" s="64" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O79" s="81">
         <v>1986</v>
@@ -6688,7 +6794,7 @@
     </row>
     <row r="80" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D80" s="71" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E80" s="86"/>
       <c r="F80" s="72" t="s">
@@ -6713,14 +6819,14 @@
     </row>
     <row r="81" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D81" s="71" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E81" s="86"/>
       <c r="F81" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G81" s="71" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H81" s="27" t="s">
         <v>85</v>
@@ -6732,24 +6838,24 @@
         <v>94</v>
       </c>
       <c r="K81" s="74" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L81" s="74" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M81" s="74"/>
       <c r="N81" s="74"/>
     </row>
     <row r="82" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="71" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E82" s="86"/>
       <c r="F82" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G82" s="71" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H82" s="27" t="s">
         <v>85</v>
@@ -6761,24 +6867,24 @@
         <v>94</v>
       </c>
       <c r="K82" s="74" t="s">
+        <v>228</v>
+      </c>
+      <c r="L82" s="74" t="s">
         <v>229</v>
-      </c>
-      <c r="L82" s="74" t="s">
-        <v>230</v>
       </c>
       <c r="M82" s="74"/>
       <c r="N82" s="74"/>
     </row>
     <row r="83" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D83" s="71" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E83" s="86"/>
       <c r="F83" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G83" s="71" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H83" s="27" t="s">
         <v>84</v>
@@ -6790,7 +6896,7 @@
         <v>102</v>
       </c>
       <c r="K83" s="74" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L83" s="74"/>
       <c r="M83" s="74"/>
@@ -6798,14 +6904,14 @@
     </row>
     <row r="84" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D84" s="68" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E84" s="85"/>
       <c r="F84" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G84" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H84" s="27" t="s">
         <v>84</v>
@@ -6817,19 +6923,19 @@
         <v>102</v>
       </c>
       <c r="K84" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="85" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D85" s="68" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E85" s="85"/>
       <c r="F85" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G85" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H85" s="27" t="s">
         <v>85</v>
@@ -6841,22 +6947,22 @@
         <v>94</v>
       </c>
       <c r="K85" t="s">
+        <v>235</v>
+      </c>
+      <c r="L85" t="s">
         <v>236</v>
-      </c>
-      <c r="L85" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="86" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D86" s="68" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E86" s="85"/>
       <c r="F86" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G86" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H86" s="27" t="s">
         <v>84</v>
@@ -6868,19 +6974,19 @@
         <v>94</v>
       </c>
       <c r="K86" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="87" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D87" s="68" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E87" s="85"/>
       <c r="F87" s="75" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G87" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H87" s="27" t="s">
         <v>85</v>
@@ -6895,19 +7001,19 @@
         <v>199</v>
       </c>
       <c r="L87" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="88" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D88" s="68" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E88" s="85"/>
       <c r="F88" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G88" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H88" s="27" t="s">
         <v>86</v>
@@ -6916,7 +7022,7 @@
         <v>91</v>
       </c>
       <c r="J88" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K88" t="s">
         <v>98</v>
@@ -6925,52 +7031,52 @@
         <v>157</v>
       </c>
       <c r="M88" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="89" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D89" s="68" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E89" s="85"/>
       <c r="F89" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G89" s="68" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H89" s="27" t="s">
         <v>87</v>
       </c>
       <c r="I89" t="s">
+        <v>243</v>
+      </c>
+      <c r="J89" t="s">
         <v>244</v>
       </c>
-      <c r="J89" t="s">
+      <c r="K89" t="s">
         <v>245</v>
       </c>
-      <c r="K89" t="s">
+      <c r="L89" t="s">
         <v>246</v>
       </c>
-      <c r="L89" t="s">
+      <c r="M89" t="s">
         <v>247</v>
       </c>
-      <c r="M89" t="s">
+      <c r="N89" t="s">
         <v>248</v>
-      </c>
-      <c r="N89" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="90" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D90" s="68" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E90" s="85"/>
       <c r="F90" s="76" t="s">
         <v>208</v>
       </c>
       <c r="G90" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H90" s="27" t="s">
         <v>85</v>
@@ -6982,22 +7088,22 @@
         <v>102</v>
       </c>
       <c r="K90" t="s">
+        <v>224</v>
+      </c>
+      <c r="L90" t="s">
         <v>225</v>
-      </c>
-      <c r="L90" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="91" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D91" s="68" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E91" s="85"/>
       <c r="F91" s="76" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G91" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H91" s="27" t="s">
         <v>85</v>
@@ -7009,22 +7115,22 @@
         <v>94</v>
       </c>
       <c r="K91" t="s">
+        <v>249</v>
+      </c>
+      <c r="L91" t="s">
         <v>250</v>
-      </c>
-      <c r="L91" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="92" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D92" s="68" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E92" s="85"/>
       <c r="F92" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G92" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H92" s="27" t="s">
         <v>86</v>
@@ -7042,19 +7148,19 @@
         <v>200</v>
       </c>
       <c r="M92" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="93" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D93" s="68" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E93" s="85"/>
       <c r="F93" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G93" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H93" s="27" t="s">
         <v>83</v>
@@ -7063,19 +7169,19 @@
         <v>89</v>
       </c>
       <c r="J93" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="94" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D94" s="68" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E94" s="85"/>
       <c r="F94" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G94" s="68" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H94" s="27" t="s">
         <v>86</v>
@@ -7093,30 +7199,30 @@
         <v>201</v>
       </c>
       <c r="M94" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="95" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D95" s="68" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E95" s="85"/>
       <c r="F95" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G95" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H95" s="27" t="s">
         <v>82</v>
       </c>
       <c r="I95" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="96" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D96" s="68" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E96" s="85"/>
       <c r="F96" s="72" t="s">
@@ -7140,14 +7246,14 @@
     </row>
     <row r="97" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D97" s="68" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E97" s="85"/>
       <c r="F97" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G97" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H97" s="27" t="s">
         <v>84</v>
@@ -7159,19 +7265,19 @@
         <v>94</v>
       </c>
       <c r="K97" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="98" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D98" s="68" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E98" s="85"/>
       <c r="F98" s="75" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G98" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H98" s="27" t="s">
         <v>84</v>
@@ -7183,19 +7289,19 @@
         <v>94</v>
       </c>
       <c r="K98" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="99" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D99" s="68" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E99" s="85"/>
       <c r="F99" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G99" s="68" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H99" s="27" t="s">
         <v>87</v>
@@ -7207,28 +7313,28 @@
         <v>102</v>
       </c>
       <c r="K99" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L99" t="s">
+        <v>258</v>
+      </c>
+      <c r="M99" t="s">
+        <v>257</v>
+      </c>
+      <c r="N99" t="s">
         <v>259</v>
-      </c>
-      <c r="M99" t="s">
-        <v>258</v>
-      </c>
-      <c r="N99" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="100" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D100" s="68" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E100" s="85"/>
       <c r="F100" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G100" s="68" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H100" s="27" t="s">
         <v>86</v>
@@ -7246,19 +7352,19 @@
         <v>193</v>
       </c>
       <c r="M100" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="101" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D101" s="68" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E101" s="85"/>
       <c r="F101" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G101" s="68" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H101" s="27" t="s">
         <v>86</v>
@@ -7270,55 +7376,55 @@
         <v>102</v>
       </c>
       <c r="K101" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L101" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="M101" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="102" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D102" s="68" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E102" s="85"/>
       <c r="F102" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G102" s="68" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H102" s="27" t="s">
         <v>86</v>
       </c>
       <c r="I102" t="s">
+        <v>264</v>
+      </c>
+      <c r="J102" t="s">
         <v>265</v>
       </c>
-      <c r="J102" t="s">
+      <c r="K102" t="s">
         <v>266</v>
       </c>
-      <c r="K102" t="s">
+      <c r="L102" t="s">
         <v>267</v>
       </c>
-      <c r="L102" t="s">
-        <v>268</v>
-      </c>
       <c r="M102" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="103" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D103" s="68" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E103" s="85"/>
       <c r="F103" s="72" t="s">
         <v>207</v>
       </c>
       <c r="G103" s="68" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H103" s="27" t="s">
         <v>87</v>
@@ -7330,28 +7436,28 @@
         <v>102</v>
       </c>
       <c r="K103" t="s">
+        <v>268</v>
+      </c>
+      <c r="L103" t="s">
         <v>269</v>
       </c>
-      <c r="L103" t="s">
+      <c r="M103" t="s">
         <v>270</v>
       </c>
-      <c r="M103" t="s">
+      <c r="N103" t="s">
         <v>271</v>
-      </c>
-      <c r="N103" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="104" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D104" s="68" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E104" s="85"/>
       <c r="F104" s="75" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G104" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H104" s="27" t="s">
         <v>85</v>
@@ -7363,22 +7469,22 @@
         <v>94</v>
       </c>
       <c r="K104" t="s">
+        <v>272</v>
+      </c>
+      <c r="L104" t="s">
         <v>273</v>
-      </c>
-      <c r="L104" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="105" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D105" s="68" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E105" s="85"/>
       <c r="F105" s="75" t="s">
         <v>207</v>
       </c>
       <c r="G105" s="68" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H105" s="27" t="s">
         <v>86</v>
@@ -7387,7 +7493,7 @@
         <v>91</v>
       </c>
       <c r="J105" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K105" t="s">
         <v>98</v>
@@ -7396,19 +7502,19 @@
         <v>157</v>
       </c>
       <c r="M105" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="106" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D106" s="68" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E106" s="85"/>
       <c r="F106" s="75" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G106" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H106" s="27" t="s">
         <v>85</v>
@@ -7420,22 +7526,22 @@
         <v>94</v>
       </c>
       <c r="K106" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L106" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="107" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D107" s="68" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E107" s="85"/>
       <c r="F107" s="75" t="s">
         <v>207</v>
       </c>
       <c r="G107" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H107" s="27" t="s">
         <v>85</v>
@@ -7447,22 +7553,22 @@
         <v>94</v>
       </c>
       <c r="K107" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L107" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="108" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D108" s="68" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E108" s="85"/>
       <c r="F108" s="75" t="s">
         <v>208</v>
       </c>
       <c r="G108" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H108" s="27" t="s">
         <v>85</v>
@@ -7474,22 +7580,22 @@
         <v>102</v>
       </c>
       <c r="K108" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L108" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="109" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D109" s="68" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E109" s="85"/>
       <c r="F109" s="75" t="s">
         <v>207</v>
       </c>
       <c r="G109" s="68" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H109" s="27" t="s">
         <v>87</v>
@@ -7501,28 +7607,28 @@
         <v>102</v>
       </c>
       <c r="K109" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L109" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="M109" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="N109" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="110" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D110" s="68" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E110" s="85"/>
       <c r="F110" s="75" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G110" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H110" s="27" t="s">
         <v>84</v>
@@ -7534,19 +7640,19 @@
         <v>94</v>
       </c>
       <c r="K110" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="111" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D111" s="68" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E111" s="85"/>
       <c r="F111" s="75" t="s">
         <v>207</v>
       </c>
       <c r="G111" s="68" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H111" s="27" t="s">
         <v>86</v>
@@ -7558,25 +7664,25 @@
         <v>102</v>
       </c>
       <c r="K111" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L111" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M111" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="112" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D112" s="68" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E112" s="85"/>
       <c r="F112" s="75" t="s">
         <v>207</v>
       </c>
       <c r="G112" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H112" s="27" t="s">
         <v>83</v>
@@ -7585,19 +7691,19 @@
         <v>89</v>
       </c>
       <c r="J112" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="113" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D113" s="68" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E113" s="85"/>
       <c r="F113" s="75" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G113" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H113" s="27" t="s">
         <v>84</v>
@@ -7609,16 +7715,16 @@
         <v>94</v>
       </c>
       <c r="K113" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="114" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D114" s="68" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E114" s="85"/>
       <c r="F114" s="75" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G114" t="s">
         <v>199</v>
@@ -7638,47 +7744,47 @@
     </row>
     <row r="115" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D115" s="68" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E115" s="85"/>
       <c r="F115" s="75" t="s">
         <v>207</v>
       </c>
       <c r="G115" s="68" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H115" s="27" t="s">
         <v>87</v>
       </c>
       <c r="I115" t="s">
+        <v>285</v>
+      </c>
+      <c r="J115" t="s">
         <v>286</v>
       </c>
-      <c r="J115" t="s">
+      <c r="K115" t="s">
         <v>287</v>
       </c>
-      <c r="K115" t="s">
+      <c r="L115" t="s">
         <v>288</v>
       </c>
-      <c r="L115" t="s">
+      <c r="M115" t="s">
         <v>289</v>
       </c>
-      <c r="M115" t="s">
+      <c r="N115" t="s">
         <v>290</v>
-      </c>
-      <c r="N115" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="116" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D116" s="68" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E116" s="85"/>
       <c r="F116" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G116" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H116" s="27" t="s">
         <v>85</v>
@@ -7693,19 +7799,19 @@
         <v>136</v>
       </c>
       <c r="L116" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="117" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D117" s="68" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E117" s="85"/>
       <c r="F117" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G117" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H117" s="27" t="s">
         <v>84</v>
@@ -7714,52 +7820,52 @@
         <v>93</v>
       </c>
       <c r="J117" t="s">
+        <v>293</v>
+      </c>
+      <c r="K117" t="s">
         <v>294</v>
-      </c>
-      <c r="K117" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="118" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D118" s="68" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E118" s="85"/>
       <c r="F118" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G118" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H118" s="27" t="s">
         <v>86</v>
       </c>
       <c r="I118" t="s">
+        <v>243</v>
+      </c>
+      <c r="J118" t="s">
         <v>244</v>
       </c>
-      <c r="J118" t="s">
-        <v>245</v>
-      </c>
       <c r="K118" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L118" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="M118" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="119" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D119" s="68" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E119" s="85"/>
       <c r="F119" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G119" s="68" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H119" s="27" t="s">
         <v>83</v>
@@ -7768,19 +7874,19 @@
         <v>93</v>
       </c>
       <c r="J119" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="120" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D120" s="68" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E120" s="85"/>
       <c r="F120" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G120" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H120" s="27" t="s">
         <v>85</v>
@@ -7792,15 +7898,15 @@
         <v>102</v>
       </c>
       <c r="K120" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L120" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="121" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D121" s="68" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E121" s="85"/>
       <c r="F121" s="77" t="s">
@@ -7818,14 +7924,14 @@
     </row>
     <row r="122" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D122" s="68" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E122" s="85"/>
       <c r="F122" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G122" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H122" s="27" t="s">
         <v>84</v>
@@ -7837,16 +7943,16 @@
         <v>102</v>
       </c>
       <c r="K122" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="123" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D123" s="68" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E123" s="85"/>
       <c r="F123" s="77" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G123" t="s">
         <v>199</v>
@@ -7866,14 +7972,14 @@
     </row>
     <row r="124" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D124" s="68" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E124" s="85"/>
       <c r="F124" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G124" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H124" s="27" t="s">
         <v>84</v>
@@ -7882,22 +7988,22 @@
         <v>93</v>
       </c>
       <c r="J124" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K124" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="125" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D125" s="68" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E125" s="85"/>
       <c r="F125" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G125" s="68" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H125" s="27" t="s">
         <v>86</v>
@@ -7915,19 +8021,19 @@
         <v>201</v>
       </c>
       <c r="M125" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="126" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D126" s="68" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E126" s="85"/>
       <c r="F126" s="77" t="s">
         <v>208</v>
       </c>
       <c r="G126" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H126" s="27" t="s">
         <v>84</v>
@@ -7939,19 +8045,19 @@
         <v>102</v>
       </c>
       <c r="K126" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="127" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D127" s="68" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E127" s="85"/>
       <c r="F127" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G127" s="68" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H127" s="27" t="s">
         <v>86</v>
@@ -7966,22 +8072,22 @@
         <v>136</v>
       </c>
       <c r="L127" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M127" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="128" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D128" s="68" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E128" s="85"/>
       <c r="F128" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G128" s="68" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H128" s="27" t="s">
         <v>86</v>
@@ -7999,19 +8105,19 @@
         <v>193</v>
       </c>
       <c r="M128" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="129" spans="4:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D129" s="68" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E129" s="85"/>
       <c r="F129" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G129" s="68" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H129" s="27" t="s">
         <v>86</v>
@@ -8026,64 +8132,64 @@
         <v>136</v>
       </c>
       <c r="L129" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M129" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="130" spans="4:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D130" s="68" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E130" s="85"/>
       <c r="F130" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G130" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H130" s="27" t="s">
         <v>83</v>
       </c>
       <c r="I130" t="s">
+        <v>243</v>
+      </c>
+      <c r="J130" t="s">
         <v>244</v>
-      </c>
-      <c r="J130" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="131" spans="4:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D131" s="68" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E131" s="85"/>
       <c r="F131" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G131" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H131" s="27" t="s">
         <v>83</v>
       </c>
       <c r="I131" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J131" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="132" spans="4:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D132" s="68" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E132" s="85"/>
       <c r="F132" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G132" s="68" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H132" s="27" t="s">
         <v>86</v>
@@ -8095,25 +8201,25 @@
         <v>102</v>
       </c>
       <c r="K132" t="s">
+        <v>224</v>
+      </c>
+      <c r="L132" t="s">
         <v>225</v>
       </c>
-      <c r="L132" t="s">
-        <v>226</v>
-      </c>
       <c r="M132" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="133" spans="4:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D133" s="68" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E133" s="85"/>
       <c r="F133" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G133" s="68" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H133" s="27" t="s">
         <v>86</v>
@@ -8128,22 +8234,22 @@
         <v>136</v>
       </c>
       <c r="L133" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M133" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="134" spans="4:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D134" s="68" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E134" s="85"/>
       <c r="F134" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G134" s="68" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H134" s="27" t="s">
         <v>86</v>
@@ -8158,22 +8264,22 @@
         <v>136</v>
       </c>
       <c r="L134" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M134" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="135" spans="4:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D135" s="68" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E135" s="85"/>
       <c r="F135" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G135" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H135" s="27" t="s">
         <v>85</v>
@@ -8182,25 +8288,25 @@
         <v>89</v>
       </c>
       <c r="J135" t="s">
+        <v>313</v>
+      </c>
+      <c r="K135" t="s">
         <v>314</v>
       </c>
-      <c r="K135" t="s">
+      <c r="L135" t="s">
         <v>315</v>
-      </c>
-      <c r="L135" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="136" spans="4:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D136" s="68" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E136" s="85"/>
       <c r="F136" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G136" s="68" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H136" s="27" t="s">
         <v>86</v>
@@ -8212,76 +8318,76 @@
         <v>102</v>
       </c>
       <c r="K136" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L136" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M136" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="137" spans="4:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D137" s="68" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E137" s="85"/>
       <c r="F137" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G137" s="68" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H137" s="27" t="s">
         <v>86</v>
       </c>
       <c r="I137" t="s">
+        <v>243</v>
+      </c>
+      <c r="J137" t="s">
         <v>244</v>
       </c>
-      <c r="J137" t="s">
-        <v>245</v>
-      </c>
       <c r="K137" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L137" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M137" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="138" spans="4:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D138" s="68" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E138" s="85"/>
       <c r="F138" s="77" t="s">
         <v>208</v>
       </c>
       <c r="G138" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H138" s="27" t="s">
         <v>83</v>
       </c>
       <c r="I138" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J138" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="139" spans="4:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D139" s="68" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E139" s="85"/>
       <c r="F139" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G139" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H139" s="27" t="s">
         <v>86</v>
@@ -8299,40 +8405,40 @@
         <v>200</v>
       </c>
       <c r="M139" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="140" spans="4:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D140" s="68" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E140" s="85"/>
       <c r="F140" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G140" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H140" s="27" t="s">
         <v>83</v>
       </c>
       <c r="I140" t="s">
+        <v>322</v>
+      </c>
+      <c r="J140" t="s">
         <v>323</v>
-      </c>
-      <c r="J140" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="141" spans="4:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D141" s="68" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E141" s="85"/>
       <c r="F141" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G141" s="68" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H141" s="27" t="s">
         <v>86</v>
@@ -8350,37 +8456,37 @@
         <v>193</v>
       </c>
       <c r="M141" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="142" spans="4:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D142" s="68" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E142" s="85"/>
       <c r="F142" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G142" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H142" s="27" t="s">
         <v>82</v>
       </c>
       <c r="I142" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="143" spans="4:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D143" s="68" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E143" s="85"/>
       <c r="F143" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G143" s="68" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H143" s="27" t="s">
         <v>86</v>
@@ -8389,7 +8495,7 @@
         <v>91</v>
       </c>
       <c r="J143" s="37" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K143" t="s">
         <v>98</v>
@@ -8398,19 +8504,19 @@
         <v>157</v>
       </c>
       <c r="M143" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="144" spans="4:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D144" s="68" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E144" s="85"/>
       <c r="F144" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G144" s="68" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H144" s="27" t="s">
         <v>86</v>
@@ -8425,24 +8531,24 @@
         <v>136</v>
       </c>
       <c r="L144" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="M144" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="145" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D145" s="68" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E145" s="85" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F145" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G145" s="68" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H145" s="27" t="s">
         <v>87</v>
@@ -8457,804 +8563,806 @@
         <v>104</v>
       </c>
       <c r="L145" t="s">
+        <v>331</v>
+      </c>
+      <c r="M145" t="s">
+        <v>330</v>
+      </c>
+      <c r="N145" t="s">
         <v>332</v>
-      </c>
-      <c r="M145" t="s">
-        <v>331</v>
-      </c>
-      <c r="N145" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="146" spans="4:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D146" s="68" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E146" s="85" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F146" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G146" s="68" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="147" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E147" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F147" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G147" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H147" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="I147" s="89" t="s">
-        <v>244</v>
+      <c r="I147" s="87" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="148" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E148" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F148" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G148" t="s">
-        <v>440</v>
-      </c>
-      <c r="H148" s="89" t="s">
-        <v>463</v>
-      </c>
-      <c r="I148" s="89" t="s">
+        <v>438</v>
+      </c>
+      <c r="H148" s="87" t="s">
+        <v>461</v>
+      </c>
+      <c r="I148" s="87" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="149" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E149" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F149" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G149" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="H149" t="s">
         <v>87</v>
       </c>
-      <c r="I149" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J149" s="89" t="s">
+      <c r="I149" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J149" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K149" s="89" t="s">
+      <c r="K149" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="L149" s="89" t="s">
+      <c r="L149" s="87" t="s">
         <v>4</v>
       </c>
       <c r="M149" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="N149" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="150" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E150" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F150" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G150" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="H150" t="s">
         <v>87</v>
       </c>
-      <c r="I150" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J150" s="89" t="s">
+      <c r="I150" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J150" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K150" s="89" t="s">
+      <c r="K150" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="L150" s="89" t="s">
+      <c r="L150" s="87" t="s">
         <v>4</v>
       </c>
       <c r="M150" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="N150" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="151" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E151" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F151" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G151" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="H151" t="s">
         <v>87</v>
       </c>
-      <c r="I151" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J151" s="89" t="s">
+      <c r="I151" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J151" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K151" s="89" t="s">
+      <c r="K151" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="L151" s="89" t="s">
+      <c r="L151" s="87" t="s">
         <v>193</v>
       </c>
       <c r="M151" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="N151" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="152" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E152" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F152" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G152" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H152" t="s">
         <v>87</v>
       </c>
-      <c r="I152" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J152" s="89" t="s">
+      <c r="I152" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J152" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K152" s="89" t="s">
+      <c r="K152" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="L152" s="89" t="s">
+      <c r="L152" s="87" t="s">
         <v>193</v>
       </c>
       <c r="M152" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="N152" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="153" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E153" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F153" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G153" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="H153" t="s">
         <v>87</v>
       </c>
-      <c r="I153" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J153" s="89" t="s">
+      <c r="I153" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J153" s="87" t="s">
         <v>135</v>
       </c>
-      <c r="K153" s="89" t="s">
+      <c r="K153" s="87" t="s">
         <v>136</v>
       </c>
-      <c r="L153" s="89" t="s">
-        <v>330</v>
+      <c r="L153" s="87" t="s">
+        <v>329</v>
       </c>
       <c r="M153" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="N153" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="154" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E154" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F154" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G154" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H154" t="s">
         <v>87</v>
       </c>
-      <c r="I154" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J154" s="89" t="s">
+      <c r="I154" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J154" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K154" s="89" t="s">
+      <c r="K154" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="L154" s="89" t="s">
+      <c r="L154" s="87" t="s">
         <v>193</v>
       </c>
       <c r="M154" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="N154" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="155" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E155" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F155" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G155" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="H155" t="s">
         <v>87</v>
       </c>
-      <c r="I155" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J155" s="89" t="s">
+      <c r="I155" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J155" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K155" s="89" t="s">
+      <c r="K155" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="L155" s="89" t="s">
+      <c r="L155" s="87" t="s">
         <v>193</v>
       </c>
       <c r="M155" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="N155" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="156" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E156" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F156" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G156" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="H156" t="s">
         <v>87</v>
       </c>
-      <c r="I156" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J156" s="89" t="s">
+      <c r="I156" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J156" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K156" s="89" t="s">
+      <c r="K156" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="L156" s="89" t="s">
+      <c r="L156" s="87" t="s">
         <v>4</v>
       </c>
       <c r="M156" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="N156" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="157" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E157" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F157" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G157" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="H157" t="s">
         <v>87</v>
       </c>
-      <c r="I157" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J157" s="89" t="s">
+      <c r="I157" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J157" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K157" s="89" t="s">
+      <c r="K157" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="L157" s="89" t="s">
+      <c r="L157" s="87" t="s">
         <v>193</v>
       </c>
       <c r="M157" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="N157" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="158" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E158" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F158" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G158" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="H158" t="s">
         <v>87</v>
       </c>
-      <c r="I158" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J158" s="89" t="s">
+      <c r="I158" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J158" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K158" s="89" t="s">
+      <c r="K158" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="L158" s="89" t="s">
+      <c r="L158" s="87" t="s">
         <v>193</v>
       </c>
       <c r="M158" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="N158" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="159" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E159" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F159" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G159" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="H159" t="s">
         <v>87</v>
       </c>
-      <c r="I159" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J159" s="89" t="s">
+      <c r="I159" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J159" s="87" t="s">
         <v>135</v>
       </c>
-      <c r="K159" s="89" t="s">
+      <c r="K159" s="87" t="s">
         <v>136</v>
       </c>
-      <c r="L159" s="89" t="s">
-        <v>330</v>
+      <c r="L159" s="87" t="s">
+        <v>329</v>
       </c>
       <c r="M159" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="N159" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="160" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E160" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="F160" s="77" t="s">
         <v>208</v>
       </c>
       <c r="G160" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="H160" t="s">
         <v>87</v>
       </c>
-      <c r="I160" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J160" s="89" t="s">
+      <c r="I160" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J160" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K160" s="89" t="s">
+      <c r="K160" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="L160" s="89" t="s">
+      <c r="L160" s="87" t="s">
         <v>193</v>
       </c>
       <c r="M160" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="N160" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="161" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E161" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F161" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G161" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="H161" t="s">
         <v>87</v>
       </c>
-      <c r="I161" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J161" s="89" t="s">
+      <c r="I161" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J161" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K161" s="89" t="s">
+      <c r="K161" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="L161" s="89" t="s">
+      <c r="L161" s="87" t="s">
         <v>4</v>
       </c>
       <c r="M161" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="N161" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="162" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E162" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F162" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G162" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="H162" t="s">
         <v>87</v>
       </c>
-      <c r="I162" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J162" s="89" t="s">
+      <c r="I162" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J162" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K162" s="89" t="s">
+      <c r="K162" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="L162" s="89" t="s">
+      <c r="L162" s="87" t="s">
         <v>193</v>
       </c>
       <c r="M162" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N162" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="163" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E163" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F163" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G163" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="H163" t="s">
         <v>87</v>
       </c>
-      <c r="I163" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J163" s="89" t="s">
+      <c r="I163" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J163" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K163" s="89" t="s">
+      <c r="K163" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="L163" s="89" t="s">
+      <c r="L163" s="87" t="s">
         <v>193</v>
       </c>
       <c r="M163" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N163" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="164" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E164" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F164" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G164" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="H164" t="s">
         <v>87</v>
       </c>
-      <c r="I164" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J164" s="89" t="s">
+      <c r="I164" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J164" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K164" s="89" t="s">
+      <c r="K164" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="L164" s="89" t="s">
+      <c r="L164" s="87" t="s">
         <v>193</v>
       </c>
       <c r="M164" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="N164" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="165" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E165" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F165" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G165" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="H165" t="s">
         <v>87</v>
       </c>
-      <c r="I165" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J165" s="89" t="s">
+      <c r="I165" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J165" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K165" s="89" t="s">
+      <c r="K165" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="L165" s="89" t="s">
+      <c r="L165" s="87" t="s">
         <v>193</v>
       </c>
       <c r="M165" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N165" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="166" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E166" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F166" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G166" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="H166" t="s">
         <v>87</v>
       </c>
-      <c r="I166" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J166" s="89" t="s">
+      <c r="I166" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J166" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K166" s="89" t="s">
+      <c r="K166" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="L166" s="89" t="s">
+      <c r="L166" s="87" t="s">
         <v>193</v>
       </c>
       <c r="M166" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="N166" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="167" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E167" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F167" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G167" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="H167" t="s">
         <v>87</v>
       </c>
-      <c r="I167" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J167" s="89" t="s">
+      <c r="I167" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J167" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K167" s="89" t="s">
+      <c r="K167" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="L167" s="89" t="s">
+      <c r="L167" s="87" t="s">
         <v>4</v>
       </c>
       <c r="M167" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="N167" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="168" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E168" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F168" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G168" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H168" t="s">
         <v>87</v>
       </c>
-      <c r="I168" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J168" s="89" t="s">
+      <c r="I168" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J168" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K168" s="89" t="s">
+      <c r="K168" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="L168" s="89" t="s">
+      <c r="L168" s="87" t="s">
         <v>193</v>
       </c>
       <c r="M168" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N168" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="169" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E169" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F169" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G169" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="H169" t="s">
         <v>87</v>
       </c>
-      <c r="I169" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J169" s="89" t="s">
+      <c r="I169" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J169" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K169" s="89" t="s">
+      <c r="K169" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="L169" s="89" t="s">
+      <c r="L169" s="87" t="s">
         <v>4</v>
       </c>
       <c r="M169" t="s">
         <v>112</v>
       </c>
       <c r="N169" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="170" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E170" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F170" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G170" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="H170" t="s">
         <v>87</v>
       </c>
-      <c r="I170" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J170" s="89" t="s">
+      <c r="I170" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J170" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K170" s="89" t="s">
+      <c r="K170" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="L170" s="89" t="s">
+      <c r="L170" s="87" t="s">
         <v>4</v>
       </c>
       <c r="M170" t="s">
         <v>112</v>
       </c>
       <c r="N170" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="171" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E171" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F171" s="77" t="s">
         <v>207</v>
       </c>
       <c r="G171" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="H171" t="s">
         <v>87</v>
       </c>
-      <c r="I171" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="J171" s="89" t="s">
+      <c r="I171" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="J171" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="K171" s="89" t="s">
+      <c r="K171" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="L171" s="89" t="s">
+      <c r="L171" s="87" t="s">
         <v>193</v>
       </c>
       <c r="M171" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="N171" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L19" r:id="rId1" tooltip="Cyclopidae" display="https://en.wikipedia.org/wiki/Cyclopidae"/>
+    <hyperlink ref="L20" r:id="rId2" tooltip="Cyclopidae" display="https://en.wikipedia.org/wiki/Cyclopidae"/>
+    <hyperlink ref="L45" r:id="rId3" tooltip="Cyclopidae" display="https://en.wikipedia.org/wiki/Cyclopidae"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Worked on adding FRP macrozoops
</commit_message>
<xml_diff>
--- a/Data/new_crosswalk.xlsx
+++ b/Data/new_crosswalk.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2985" uniqueCount="764">
   <si>
     <t>ACARTELA</t>
   </si>
@@ -1698,6 +1698,708 @@
   </si>
   <si>
     <t>Calanoid</t>
+  </si>
+  <si>
+    <t>Cyclopoid UNID</t>
+  </si>
+  <si>
+    <t>Cyclopoid</t>
+  </si>
+  <si>
+    <t>Homocyclops</t>
+  </si>
+  <si>
+    <t>Copepod UNID</t>
+  </si>
+  <si>
+    <t>Parasitic Copepod</t>
+  </si>
+  <si>
+    <t>Hydrophilidae Larvae Beetle</t>
+  </si>
+  <si>
+    <t>Hydrophilide</t>
+  </si>
+  <si>
+    <t>Hydrophilidae Adult Beetle</t>
+  </si>
+  <si>
+    <t>Coleoptera Other</t>
+  </si>
+  <si>
+    <t>Dytiscidae larvae</t>
+  </si>
+  <si>
+    <t>Dytiscidae</t>
+  </si>
+  <si>
+    <t>Staphylinidae adult</t>
+  </si>
+  <si>
+    <t>Staphylinidae</t>
+  </si>
+  <si>
+    <t>Curculionidae</t>
+  </si>
+  <si>
+    <t>Noteridae</t>
+  </si>
+  <si>
+    <t>Dytiscidae adult</t>
+  </si>
+  <si>
+    <t>Elmidae</t>
+  </si>
+  <si>
+    <t>Elmidae larvae</t>
+  </si>
+  <si>
+    <t>Gyrinidae larvae</t>
+  </si>
+  <si>
+    <t>Gyrinidae</t>
+  </si>
+  <si>
+    <t>Curculionidae Larvae</t>
+  </si>
+  <si>
+    <t>Chrysomelidae Adult</t>
+  </si>
+  <si>
+    <t>Chrysomelidae</t>
+  </si>
+  <si>
+    <t>Scolytinae Adult</t>
+  </si>
+  <si>
+    <t>Scolytus</t>
+  </si>
+  <si>
+    <t>Haliplidae Larvae</t>
+  </si>
+  <si>
+    <t>Haliplidae</t>
+  </si>
+  <si>
+    <t>Carabidae Larvae</t>
+  </si>
+  <si>
+    <t>Carabidae</t>
+  </si>
+  <si>
+    <t>Hydraenidae</t>
+  </si>
+  <si>
+    <t>Hydraenidea</t>
+  </si>
+  <si>
+    <t>Coccinellidae Adult</t>
+  </si>
+  <si>
+    <t>Coccinellidae</t>
+  </si>
+  <si>
+    <t>Ptilidae</t>
+  </si>
+  <si>
+    <t>Hydroscaphidae Adult</t>
+  </si>
+  <si>
+    <t>Hydroscaphidae</t>
+  </si>
+  <si>
+    <t>Tenebrionidae adult</t>
+  </si>
+  <si>
+    <t>Tenebrionidae</t>
+  </si>
+  <si>
+    <t>Coccinellidae Larvae</t>
+  </si>
+  <si>
+    <t>Scirtidae adult</t>
+  </si>
+  <si>
+    <t>Scirtidae</t>
+  </si>
+  <si>
+    <t>Earwig</t>
+  </si>
+  <si>
+    <t>Dermaptera</t>
+  </si>
+  <si>
+    <t>Ephydridae Larvae</t>
+  </si>
+  <si>
+    <t>Ephydridae</t>
+  </si>
+  <si>
+    <t>Brachycera Larvae</t>
+  </si>
+  <si>
+    <t>Diptera Larvae Other</t>
+  </si>
+  <si>
+    <t>Brachycera Pupae</t>
+  </si>
+  <si>
+    <t>Psychodidae larvae</t>
+  </si>
+  <si>
+    <t>Psychodidae</t>
+  </si>
+  <si>
+    <t>Tabanidae</t>
+  </si>
+  <si>
+    <t>Nematocera pupae</t>
+  </si>
+  <si>
+    <t>Dolichopodidae larvae</t>
+  </si>
+  <si>
+    <t>Dolichopodidae</t>
+  </si>
+  <si>
+    <t>Tipulidae larvae</t>
+  </si>
+  <si>
+    <t>Tipulidae</t>
+  </si>
+  <si>
+    <t>Sciomyzidae Larvae</t>
+  </si>
+  <si>
+    <t>Sciomyzidae</t>
+  </si>
+  <si>
+    <t>Culicidae Larvae</t>
+  </si>
+  <si>
+    <t>Culicidae</t>
+  </si>
+  <si>
+    <t>Simuliidae larvae</t>
+  </si>
+  <si>
+    <t>Simuliidae</t>
+  </si>
+  <si>
+    <t>Muscidae larvae</t>
+  </si>
+  <si>
+    <t>Muscidae</t>
+  </si>
+  <si>
+    <t>Stratiomyidae larvae</t>
+  </si>
+  <si>
+    <t>Stratiomyidae</t>
+  </si>
+  <si>
+    <t>Baetidae</t>
+  </si>
+  <si>
+    <t>Caenidae</t>
+  </si>
+  <si>
+    <t>Ephemeroptera larvae Other</t>
+  </si>
+  <si>
+    <t>Tricorythidae larvae</t>
+  </si>
+  <si>
+    <t>Tricorythidae</t>
+  </si>
+  <si>
+    <t>Leptohyphidae mayfly larvae</t>
+  </si>
+  <si>
+    <t>Leptohyphidae</t>
+  </si>
+  <si>
+    <t>Tricorythodes</t>
+  </si>
+  <si>
+    <t>minutus</t>
+  </si>
+  <si>
+    <t>Tricorythodes minutus</t>
+  </si>
+  <si>
+    <t>Ephemeroptera Adult</t>
+  </si>
+  <si>
+    <t>Belostomatidae</t>
+  </si>
+  <si>
+    <t>Gerridae</t>
+  </si>
+  <si>
+    <t>Hydrometridae</t>
+  </si>
+  <si>
+    <t>Mesoveliidae</t>
+  </si>
+  <si>
+    <t>Vellidae</t>
+  </si>
+  <si>
+    <t>Hemiptera Other</t>
+  </si>
+  <si>
+    <t>Hebridae</t>
+  </si>
+  <si>
+    <t>Nepidae</t>
+  </si>
+  <si>
+    <t>Homoptera</t>
+  </si>
+  <si>
+    <t>Leafhopper</t>
+  </si>
+  <si>
+    <t>Cicadellidae</t>
+  </si>
+  <si>
+    <t>juvenile leafhopper</t>
+  </si>
+  <si>
+    <t>Psyllidae Larvae</t>
+  </si>
+  <si>
+    <t>Hymenoptera Other</t>
+  </si>
+  <si>
+    <t>Lepidoptera Larvae</t>
+  </si>
+  <si>
+    <t>Lepidoptera</t>
+  </si>
+  <si>
+    <t>Lepidoptera adult</t>
+  </si>
+  <si>
+    <t>Lepidoptera pupae</t>
+  </si>
+  <si>
+    <t>Sisyridae Larvae</t>
+  </si>
+  <si>
+    <t>Neuroptera</t>
+  </si>
+  <si>
+    <t>Sisyridae</t>
+  </si>
+  <si>
+    <t>Gomphidae larvae</t>
+  </si>
+  <si>
+    <t>Odanata</t>
+  </si>
+  <si>
+    <t>Gompidae</t>
+  </si>
+  <si>
+    <t>Zygoptera Adult</t>
+  </si>
+  <si>
+    <t>Aeshnidae larvae</t>
+  </si>
+  <si>
+    <t>Aeshnidae</t>
+  </si>
+  <si>
+    <t>Odonata larvae Other</t>
+  </si>
+  <si>
+    <t>Libellulidae</t>
+  </si>
+  <si>
+    <t>Orthoptera</t>
+  </si>
+  <si>
+    <t>Psocoptera Adult</t>
+  </si>
+  <si>
+    <t>Psocoptera</t>
+  </si>
+  <si>
+    <t>Psocoptera Larvae</t>
+  </si>
+  <si>
+    <t>Tricoptera larvae Other</t>
+  </si>
+  <si>
+    <t>Hydroptilidae Adult Caddisfly</t>
+  </si>
+  <si>
+    <t>Polycentripodidae larvae</t>
+  </si>
+  <si>
+    <t>Polycentripodidae</t>
+  </si>
+  <si>
+    <t>Trichoptera Adult</t>
+  </si>
+  <si>
+    <t>Hydroptilidae Pupae Caddisfly</t>
+  </si>
+  <si>
+    <t>Insect larvae Other</t>
+  </si>
+  <si>
+    <t>Juvenile Amphipod</t>
+  </si>
+  <si>
+    <t>Melita</t>
+  </si>
+  <si>
+    <t>Hadzioidea</t>
+  </si>
+  <si>
+    <t>Ampithoe</t>
+  </si>
+  <si>
+    <t>Ampithoidae</t>
+  </si>
+  <si>
+    <t>Corophium alienense</t>
+  </si>
+  <si>
+    <t>Eogammarus</t>
+  </si>
+  <si>
+    <t>Anisogammaridae</t>
+  </si>
+  <si>
+    <t>Talitridae</t>
+  </si>
+  <si>
+    <t>malacostraca</t>
+  </si>
+  <si>
+    <t>Crab megalope</t>
+  </si>
+  <si>
+    <t>Exopalaemon</t>
+  </si>
+  <si>
+    <t>Palaemonidae</t>
+  </si>
+  <si>
+    <t>modestus</t>
+  </si>
+  <si>
+    <t>Exopalaemon modestus</t>
+  </si>
+  <si>
+    <t>Shrimp Other</t>
+  </si>
+  <si>
+    <t>Crayfish</t>
+  </si>
+  <si>
+    <t>Astacidae</t>
+  </si>
+  <si>
+    <t>Pacifastacus</t>
+  </si>
+  <si>
+    <t>Palaemonetes</t>
+  </si>
+  <si>
+    <t>Juvenile Shrimp</t>
+  </si>
+  <si>
+    <t>Crangon</t>
+  </si>
+  <si>
+    <t>Crangonidae</t>
+  </si>
+  <si>
+    <t>Harris Mud Crab</t>
+  </si>
+  <si>
+    <t>Rhithropanopeus</t>
+  </si>
+  <si>
+    <t>harrisii</t>
+  </si>
+  <si>
+    <t>Rhithropanopeus harrisii</t>
+  </si>
+  <si>
+    <t>Mississippi Grass Shrimp</t>
+  </si>
+  <si>
+    <t>Palaemon</t>
+  </si>
+  <si>
+    <t>Asellidae</t>
+  </si>
+  <si>
+    <t>Ligidium</t>
+  </si>
+  <si>
+    <t>Ligiidae</t>
+  </si>
+  <si>
+    <t>lates??</t>
+  </si>
+  <si>
+    <t>Ligidium lates??</t>
+  </si>
+  <si>
+    <t>Caecidotea</t>
+  </si>
+  <si>
+    <t>Munnidae</t>
+  </si>
+  <si>
+    <t>Isopod other</t>
+  </si>
+  <si>
+    <t>Juvenile Isopod</t>
+  </si>
+  <si>
+    <t>Acanthomysis bowmani</t>
+  </si>
+  <si>
+    <t>Hyperacanthomysis longirostris</t>
+  </si>
+  <si>
+    <t>longirostris</t>
+  </si>
+  <si>
+    <t>Hyperacanthomysis</t>
+  </si>
+  <si>
+    <t>Acanthomysis hwanhaiensis</t>
+  </si>
+  <si>
+    <t>Orientomysis hwanhaiensis</t>
+  </si>
+  <si>
+    <t>hwanhaiensis</t>
+  </si>
+  <si>
+    <t>Acanthomysis macropsis</t>
+  </si>
+  <si>
+    <t>Alienacanthomysis macropsis</t>
+  </si>
+  <si>
+    <t>Alienacanthomysis</t>
+  </si>
+  <si>
+    <t>macropsis</t>
+  </si>
+  <si>
+    <t>Deltamysis homquistae</t>
+  </si>
+  <si>
+    <t>Deltamysis holmquistae</t>
+  </si>
+  <si>
+    <t>Deltamysis</t>
+  </si>
+  <si>
+    <t>holmquistae</t>
+  </si>
+  <si>
+    <t>Mysid Other</t>
+  </si>
+  <si>
+    <t>Juvenile Mysid</t>
+  </si>
+  <si>
+    <t>Malcostraca Other</t>
+  </si>
+  <si>
+    <t>Magnificent Bryozoan</t>
+  </si>
+  <si>
+    <t>Bryozoa</t>
+  </si>
+  <si>
+    <t>Phylactolaemata</t>
+  </si>
+  <si>
+    <t>Plumatellida</t>
+  </si>
+  <si>
+    <t>Pectinatellidae</t>
+  </si>
+  <si>
+    <t>Pectinatella</t>
+  </si>
+  <si>
+    <t>Pectinatella magnifica</t>
+  </si>
+  <si>
+    <t>magnifica</t>
+  </si>
+  <si>
+    <t>Cnidaria Other</t>
+  </si>
+  <si>
+    <t>Aequorea spp.</t>
+  </si>
+  <si>
+    <t>Aequoreidae</t>
+  </si>
+  <si>
+    <t>Aequorea</t>
+  </si>
+  <si>
+    <t>Leptothecata</t>
+  </si>
+  <si>
+    <t>Jellyfish Unid</t>
+  </si>
+  <si>
+    <t>Maeotias</t>
+  </si>
+  <si>
+    <t>Olindiidae</t>
+  </si>
+  <si>
+    <t>Limnomedusae</t>
+  </si>
+  <si>
+    <t>Moon Jellyfish</t>
+  </si>
+  <si>
+    <t>Ulmaridae</t>
+  </si>
+  <si>
+    <t>Aurelia</t>
+  </si>
+  <si>
+    <t>Scyphozoa</t>
+  </si>
+  <si>
+    <t>Semaeostomeae</t>
+  </si>
+  <si>
+    <t>Potamocorbula</t>
+  </si>
+  <si>
+    <t>Myoida</t>
+  </si>
+  <si>
+    <t>Corbulidae</t>
+  </si>
+  <si>
+    <t>amurensis</t>
+  </si>
+  <si>
+    <t>Potamocorbula amurensis</t>
+  </si>
+  <si>
+    <t>Juvenile Clam</t>
+  </si>
+  <si>
+    <t>Corbicula</t>
+  </si>
+  <si>
+    <t>Veneroida</t>
+  </si>
+  <si>
+    <t>Corbiculidae</t>
+  </si>
+  <si>
+    <t>fluminea</t>
+  </si>
+  <si>
+    <t>Corbicula fluminea</t>
+  </si>
+  <si>
+    <t>Clam Other</t>
+  </si>
+  <si>
+    <t>Fluminicola</t>
+  </si>
+  <si>
+    <t>Gastopoda</t>
+  </si>
+  <si>
+    <t>Lythoglyphidae</t>
+  </si>
+  <si>
+    <t>Littorinimorpha</t>
+  </si>
+  <si>
+    <t>Fossaria</t>
+  </si>
+  <si>
+    <t>Basommatophora</t>
+  </si>
+  <si>
+    <t>Lymnaeidae</t>
+  </si>
+  <si>
+    <t>Lymnaea</t>
+  </si>
+  <si>
+    <t>Hydrobiidae</t>
+  </si>
+  <si>
+    <t>Nudibranch</t>
+  </si>
+  <si>
+    <t>Nudibranchia</t>
+  </si>
+  <si>
+    <t>Melanoides tuberculata</t>
+  </si>
+  <si>
+    <t>Thiaridae</t>
+  </si>
+  <si>
+    <t>Melanoides</t>
+  </si>
+  <si>
+    <t>tuberculata</t>
+  </si>
+  <si>
+    <t>Caenogastropoda</t>
+  </si>
+  <si>
+    <t>Snail Other</t>
+  </si>
+  <si>
+    <t>Planorbella</t>
+  </si>
+  <si>
+    <t>Hygrophila</t>
+  </si>
+  <si>
+    <t>Planorbidae UNID</t>
+  </si>
+  <si>
+    <t>Slug</t>
+  </si>
+  <si>
+    <t>Prostoma</t>
+  </si>
+  <si>
+    <t>Nemertea</t>
+  </si>
+  <si>
+    <t>Enopla</t>
+  </si>
+  <si>
+    <t>Monostilifera</t>
+  </si>
+  <si>
+    <t>Tetrastemmatidae</t>
+  </si>
+  <si>
+    <t>Animal material UNID</t>
   </si>
 </sst>
 </file>
@@ -3120,11 +3822,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V182"/>
+  <dimension ref="A1:V314"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T21" sqref="T21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A283" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G313" sqref="G313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4143,7 +4845,7 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
         <v>19</v>
       </c>
@@ -4153,6 +4855,9 @@
       <c r="C23" s="30" t="s">
         <v>20</v>
       </c>
+      <c r="D23" t="s">
+        <v>20</v>
+      </c>
       <c r="F23" s="30" t="s">
         <v>207</v>
       </c>
@@ -4193,7 +4898,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
         <v>21</v>
       </c>
@@ -4203,6 +4908,9 @@
       <c r="C24" s="30" t="s">
         <v>22</v>
       </c>
+      <c r="D24" t="s">
+        <v>22</v>
+      </c>
       <c r="E24" s="30" t="s">
         <v>398</v>
       </c>
@@ -4246,7 +4954,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>23</v>
       </c>
@@ -4256,6 +4964,9 @@
       <c r="C25" s="30" t="s">
         <v>24</v>
       </c>
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
       <c r="F25" s="30" t="s">
         <v>207</v>
       </c>
@@ -4296,7 +5007,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>25</v>
       </c>
@@ -4304,6 +5015,9 @@
         <v>25</v>
       </c>
       <c r="C26" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" t="s">
         <v>26</v>
       </c>
       <c r="F26" s="30" t="s">
@@ -4384,12 +5098,12 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="C28" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="D28" s="30" t="s">
-        <v>339</v>
+      <c r="D28" t="s">
+        <v>530</v>
       </c>
       <c r="E28" s="30" t="s">
         <v>381</v>
@@ -4423,6 +5137,9 @@
       <c r="C29" s="30" t="s">
         <v>108</v>
       </c>
+      <c r="D29" s="30" t="s">
+        <v>339</v>
+      </c>
       <c r="E29" s="30" t="s">
         <v>397</v>
       </c>
@@ -4454,11 +5171,14 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>500</v>
       </c>
       <c r="B30" s="31"/>
+      <c r="D30" t="s">
+        <v>531</v>
+      </c>
       <c r="F30" s="30" t="s">
         <v>207</v>
       </c>
@@ -6081,13 +6801,16 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="31" t="s">
         <v>77</v>
       </c>
       <c r="C71" s="30" t="s">
         <v>78</v>
       </c>
+      <c r="D71" t="s">
+        <v>78</v>
+      </c>
       <c r="F71" s="30" t="s">
         <v>207</v>
       </c>
@@ -6119,7 +6842,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="31" t="s">
         <v>61</v>
       </c>
@@ -6127,6 +6850,9 @@
         <v>61</v>
       </c>
       <c r="C72" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="D72" t="s">
         <v>159</v>
       </c>
       <c r="F72" s="30" t="s">
@@ -6201,7 +6927,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="30" t="s">
         <v>64</v>
       </c>
@@ -6209,6 +6935,9 @@
         <v>64</v>
       </c>
       <c r="C74" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D74" t="s">
         <v>143</v>
       </c>
       <c r="F74" s="30" t="s">
@@ -6408,8 +7137,11 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="C80" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D80" t="s">
         <v>219</v>
       </c>
       <c r="F80" s="30" t="s">
@@ -8981,10 +9713,13 @@
         <v>518</v>
       </c>
     </row>
-    <row r="174" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B174" s="32" t="s">
         <v>503</v>
       </c>
+      <c r="D174" t="s">
+        <v>512</v>
+      </c>
       <c r="F174" s="30" t="s">
         <v>207</v>
       </c>
@@ -9013,10 +9748,13 @@
         <v>519</v>
       </c>
     </row>
-    <row r="175" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B175" s="32" t="s">
         <v>504</v>
       </c>
+      <c r="D175" t="s">
+        <v>513</v>
+      </c>
       <c r="F175" s="30" t="s">
         <v>207</v>
       </c>
@@ -9045,9 +9783,12 @@
         <v>520</v>
       </c>
     </row>
-    <row r="176" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B176" s="32" t="s">
         <v>505</v>
+      </c>
+      <c r="D176" t="s">
+        <v>652</v>
       </c>
       <c r="F176" s="30" t="s">
         <v>207</v>
@@ -9189,6 +9930,3400 @@
       </c>
       <c r="H182" s="30" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="183" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D183" t="s">
+        <v>472</v>
+      </c>
+      <c r="F183" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G183" t="s">
+        <v>472</v>
+      </c>
+      <c r="H183" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I183" t="s">
+        <v>93</v>
+      </c>
+      <c r="J183" t="s">
+        <v>101</v>
+      </c>
+      <c r="K183" t="s">
+        <v>104</v>
+      </c>
+      <c r="L183" t="s">
+        <v>193</v>
+      </c>
+      <c r="M183" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="184" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D184" t="s">
+        <v>532</v>
+      </c>
+      <c r="F184" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G184" t="s">
+        <v>532</v>
+      </c>
+      <c r="H184" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I184" t="s">
+        <v>93</v>
+      </c>
+      <c r="J184" t="s">
+        <v>101</v>
+      </c>
+      <c r="K184" t="s">
+        <v>104</v>
+      </c>
+      <c r="L184" t="s">
+        <v>193</v>
+      </c>
+      <c r="M184" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="185" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D185" t="s">
+        <v>467</v>
+      </c>
+      <c r="F185" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G185" t="s">
+        <v>467</v>
+      </c>
+      <c r="H185" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I185" t="s">
+        <v>93</v>
+      </c>
+      <c r="J185" t="s">
+        <v>101</v>
+      </c>
+      <c r="K185" t="s">
+        <v>104</v>
+      </c>
+      <c r="L185" t="s">
+        <v>193</v>
+      </c>
+      <c r="M185" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="186" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D186" t="s">
+        <v>533</v>
+      </c>
+      <c r="F186" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G186" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="H186" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="I186" t="s">
+        <v>93</v>
+      </c>
+      <c r="J186" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="187" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D187" t="s">
+        <v>534</v>
+      </c>
+      <c r="F187" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G187" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="H187" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="I187" t="s">
+        <v>93</v>
+      </c>
+      <c r="J187" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="188" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D188" t="s">
+        <v>535</v>
+      </c>
+      <c r="F188" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G188" t="s">
+        <v>536</v>
+      </c>
+      <c r="H188" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I188" t="s">
+        <v>93</v>
+      </c>
+      <c r="J188" t="s">
+        <v>94</v>
+      </c>
+      <c r="K188" t="s">
+        <v>278</v>
+      </c>
+      <c r="L188" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="189" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D189" t="s">
+        <v>537</v>
+      </c>
+      <c r="F189" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G189" t="s">
+        <v>536</v>
+      </c>
+      <c r="H189" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I189" t="s">
+        <v>93</v>
+      </c>
+      <c r="J189" t="s">
+        <v>94</v>
+      </c>
+      <c r="K189" t="s">
+        <v>278</v>
+      </c>
+      <c r="L189" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="190" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D190" t="s">
+        <v>538</v>
+      </c>
+      <c r="F190" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G190" t="s">
+        <v>278</v>
+      </c>
+      <c r="H190" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I190" t="s">
+        <v>93</v>
+      </c>
+      <c r="J190" t="s">
+        <v>94</v>
+      </c>
+      <c r="K190" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="191" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D191" t="s">
+        <v>539</v>
+      </c>
+      <c r="F191" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G191" t="s">
+        <v>540</v>
+      </c>
+      <c r="H191" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I191" t="s">
+        <v>93</v>
+      </c>
+      <c r="J191" t="s">
+        <v>94</v>
+      </c>
+      <c r="K191" t="s">
+        <v>278</v>
+      </c>
+      <c r="L191" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="192" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D192" t="s">
+        <v>541</v>
+      </c>
+      <c r="F192" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G192" t="s">
+        <v>542</v>
+      </c>
+      <c r="H192" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I192" t="s">
+        <v>93</v>
+      </c>
+      <c r="J192" t="s">
+        <v>94</v>
+      </c>
+      <c r="K192" t="s">
+        <v>278</v>
+      </c>
+      <c r="L192" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="193" spans="4:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D193" t="s">
+        <v>543</v>
+      </c>
+      <c r="F193" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G193" t="s">
+        <v>543</v>
+      </c>
+      <c r="H193" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I193" t="s">
+        <v>93</v>
+      </c>
+      <c r="J193" t="s">
+        <v>94</v>
+      </c>
+      <c r="K193" t="s">
+        <v>278</v>
+      </c>
+      <c r="L193" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="194" spans="4:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D194" t="s">
+        <v>544</v>
+      </c>
+      <c r="F194" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G194" t="s">
+        <v>544</v>
+      </c>
+      <c r="H194" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I194" t="s">
+        <v>93</v>
+      </c>
+      <c r="J194" t="s">
+        <v>94</v>
+      </c>
+      <c r="K194" t="s">
+        <v>278</v>
+      </c>
+      <c r="L194" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="195" spans="4:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D195" s="30" t="s">
+        <v>545</v>
+      </c>
+      <c r="F195" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G195" t="s">
+        <v>540</v>
+      </c>
+      <c r="H195" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I195" t="s">
+        <v>93</v>
+      </c>
+      <c r="J195" t="s">
+        <v>94</v>
+      </c>
+      <c r="K195" t="s">
+        <v>278</v>
+      </c>
+      <c r="L195" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="196" spans="4:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D196" t="s">
+        <v>546</v>
+      </c>
+      <c r="F196" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G196" t="s">
+        <v>546</v>
+      </c>
+      <c r="H196" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I196" t="s">
+        <v>93</v>
+      </c>
+      <c r="J196" t="s">
+        <v>94</v>
+      </c>
+      <c r="K196" t="s">
+        <v>278</v>
+      </c>
+      <c r="L196" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="197" spans="4:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D197" t="s">
+        <v>547</v>
+      </c>
+      <c r="F197" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G197" t="s">
+        <v>546</v>
+      </c>
+      <c r="H197" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I197" t="s">
+        <v>93</v>
+      </c>
+      <c r="J197" t="s">
+        <v>94</v>
+      </c>
+      <c r="K197" t="s">
+        <v>278</v>
+      </c>
+      <c r="L197" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="198" spans="4:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D198" t="s">
+        <v>548</v>
+      </c>
+      <c r="F198" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G198" t="s">
+        <v>549</v>
+      </c>
+      <c r="H198" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I198" t="s">
+        <v>93</v>
+      </c>
+      <c r="J198" t="s">
+        <v>94</v>
+      </c>
+      <c r="K198" t="s">
+        <v>278</v>
+      </c>
+      <c r="L198" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="199" spans="4:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D199" t="s">
+        <v>550</v>
+      </c>
+      <c r="F199" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G199" t="s">
+        <v>543</v>
+      </c>
+      <c r="H199" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I199" t="s">
+        <v>93</v>
+      </c>
+      <c r="J199" t="s">
+        <v>94</v>
+      </c>
+      <c r="K199" t="s">
+        <v>278</v>
+      </c>
+      <c r="L199" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="200" spans="4:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D200" t="s">
+        <v>551</v>
+      </c>
+      <c r="F200" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G200" t="s">
+        <v>552</v>
+      </c>
+      <c r="H200" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I200" t="s">
+        <v>93</v>
+      </c>
+      <c r="J200" t="s">
+        <v>94</v>
+      </c>
+      <c r="K200" t="s">
+        <v>278</v>
+      </c>
+      <c r="L200" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="201" spans="4:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D201" t="s">
+        <v>553</v>
+      </c>
+      <c r="F201" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G201" t="s">
+        <v>554</v>
+      </c>
+      <c r="H201" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I201" t="s">
+        <v>93</v>
+      </c>
+      <c r="J201" t="s">
+        <v>94</v>
+      </c>
+      <c r="K201" t="s">
+        <v>278</v>
+      </c>
+      <c r="L201" t="s">
+        <v>543</v>
+      </c>
+      <c r="M201" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="202" spans="4:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D202" t="s">
+        <v>555</v>
+      </c>
+      <c r="F202" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G202" t="s">
+        <v>556</v>
+      </c>
+      <c r="H202" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I202" t="s">
+        <v>93</v>
+      </c>
+      <c r="J202" t="s">
+        <v>94</v>
+      </c>
+      <c r="K202" t="s">
+        <v>278</v>
+      </c>
+      <c r="L202" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="203" spans="4:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D203" t="s">
+        <v>557</v>
+      </c>
+      <c r="F203" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G203" t="s">
+        <v>558</v>
+      </c>
+      <c r="H203" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I203" t="s">
+        <v>93</v>
+      </c>
+      <c r="J203" t="s">
+        <v>94</v>
+      </c>
+      <c r="K203" t="s">
+        <v>278</v>
+      </c>
+      <c r="L203" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="204" spans="4:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D204" t="s">
+        <v>559</v>
+      </c>
+      <c r="F204" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G204" t="s">
+        <v>560</v>
+      </c>
+      <c r="H204" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I204" t="s">
+        <v>93</v>
+      </c>
+      <c r="J204" t="s">
+        <v>94</v>
+      </c>
+      <c r="K204" t="s">
+        <v>278</v>
+      </c>
+      <c r="L204" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="205" spans="4:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D205" t="s">
+        <v>561</v>
+      </c>
+      <c r="F205" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G205" t="s">
+        <v>562</v>
+      </c>
+      <c r="H205" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I205" t="s">
+        <v>93</v>
+      </c>
+      <c r="J205" t="s">
+        <v>94</v>
+      </c>
+      <c r="K205" t="s">
+        <v>278</v>
+      </c>
+      <c r="L205" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="206" spans="4:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D206" t="s">
+        <v>563</v>
+      </c>
+      <c r="F206" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G206" t="s">
+        <v>563</v>
+      </c>
+      <c r="H206" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I206" t="s">
+        <v>93</v>
+      </c>
+      <c r="J206" t="s">
+        <v>94</v>
+      </c>
+      <c r="K206" t="s">
+        <v>278</v>
+      </c>
+      <c r="L206" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="207" spans="4:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D207" t="s">
+        <v>564</v>
+      </c>
+      <c r="F207" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G207" t="s">
+        <v>565</v>
+      </c>
+      <c r="H207" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I207" t="s">
+        <v>93</v>
+      </c>
+      <c r="J207" t="s">
+        <v>94</v>
+      </c>
+      <c r="K207" t="s">
+        <v>278</v>
+      </c>
+      <c r="L207" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="208" spans="4:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D208" t="s">
+        <v>566</v>
+      </c>
+      <c r="F208" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G208" t="s">
+        <v>567</v>
+      </c>
+      <c r="H208" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I208" t="s">
+        <v>93</v>
+      </c>
+      <c r="J208" t="s">
+        <v>94</v>
+      </c>
+      <c r="K208" t="s">
+        <v>278</v>
+      </c>
+      <c r="L208" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="209" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D209" t="s">
+        <v>568</v>
+      </c>
+      <c r="F209" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G209" t="s">
+        <v>562</v>
+      </c>
+      <c r="H209" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I209" t="s">
+        <v>93</v>
+      </c>
+      <c r="J209" t="s">
+        <v>94</v>
+      </c>
+      <c r="K209" t="s">
+        <v>278</v>
+      </c>
+      <c r="L209" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="210" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D210" t="s">
+        <v>569</v>
+      </c>
+      <c r="F210" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G210" t="s">
+        <v>570</v>
+      </c>
+      <c r="H210" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I210" t="s">
+        <v>93</v>
+      </c>
+      <c r="J210" t="s">
+        <v>94</v>
+      </c>
+      <c r="K210" t="s">
+        <v>278</v>
+      </c>
+      <c r="L210" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="211" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D211" t="s">
+        <v>571</v>
+      </c>
+      <c r="F211" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G211" t="s">
+        <v>572</v>
+      </c>
+      <c r="H211" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I211" t="s">
+        <v>93</v>
+      </c>
+      <c r="J211" t="s">
+        <v>94</v>
+      </c>
+      <c r="K211" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="212" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D212" t="s">
+        <v>573</v>
+      </c>
+      <c r="F212" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G212" t="s">
+        <v>574</v>
+      </c>
+      <c r="H212" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I212" t="s">
+        <v>93</v>
+      </c>
+      <c r="J212" t="s">
+        <v>94</v>
+      </c>
+      <c r="K212" t="s">
+        <v>199</v>
+      </c>
+      <c r="L212" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="213" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D213" t="s">
+        <v>575</v>
+      </c>
+      <c r="F213" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G213" t="s">
+        <v>199</v>
+      </c>
+      <c r="H213" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I213" t="s">
+        <v>93</v>
+      </c>
+      <c r="J213" t="s">
+        <v>94</v>
+      </c>
+      <c r="K213" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="214" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D214" t="s">
+        <v>576</v>
+      </c>
+      <c r="F214" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G214" t="s">
+        <v>199</v>
+      </c>
+      <c r="H214" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I214" t="s">
+        <v>93</v>
+      </c>
+      <c r="J214" t="s">
+        <v>94</v>
+      </c>
+      <c r="K214" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="215" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D215" t="s">
+        <v>577</v>
+      </c>
+      <c r="F215" s="30" t="s">
+        <v>298</v>
+      </c>
+      <c r="G215" t="s">
+        <v>199</v>
+      </c>
+      <c r="H215" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I215" t="s">
+        <v>93</v>
+      </c>
+      <c r="J215" t="s">
+        <v>94</v>
+      </c>
+      <c r="K215" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="216" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D216" t="s">
+        <v>578</v>
+      </c>
+      <c r="F216" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G216" t="s">
+        <v>579</v>
+      </c>
+      <c r="H216" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I216" t="s">
+        <v>93</v>
+      </c>
+      <c r="J216" t="s">
+        <v>94</v>
+      </c>
+      <c r="K216" t="s">
+        <v>199</v>
+      </c>
+      <c r="L216" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="217" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D217" t="s">
+        <v>580</v>
+      </c>
+      <c r="F217" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G217" t="s">
+        <v>580</v>
+      </c>
+      <c r="H217" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I217" t="s">
+        <v>93</v>
+      </c>
+      <c r="J217" t="s">
+        <v>94</v>
+      </c>
+      <c r="K217" t="s">
+        <v>199</v>
+      </c>
+      <c r="L217" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="218" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D218" t="s">
+        <v>581</v>
+      </c>
+      <c r="F218" s="30" t="s">
+        <v>298</v>
+      </c>
+      <c r="G218" t="s">
+        <v>199</v>
+      </c>
+      <c r="H218" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I218" t="s">
+        <v>93</v>
+      </c>
+      <c r="J218" t="s">
+        <v>94</v>
+      </c>
+      <c r="K218" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="219" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D219" t="s">
+        <v>582</v>
+      </c>
+      <c r="F219" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G219" t="s">
+        <v>583</v>
+      </c>
+      <c r="H219" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I219" t="s">
+        <v>93</v>
+      </c>
+      <c r="J219" t="s">
+        <v>94</v>
+      </c>
+      <c r="K219" t="s">
+        <v>199</v>
+      </c>
+      <c r="L219" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="220" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D220" t="s">
+        <v>584</v>
+      </c>
+      <c r="F220" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G220" t="s">
+        <v>585</v>
+      </c>
+      <c r="H220" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I220" t="s">
+        <v>93</v>
+      </c>
+      <c r="J220" t="s">
+        <v>94</v>
+      </c>
+      <c r="K220" t="s">
+        <v>199</v>
+      </c>
+      <c r="L220" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="221" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D221" t="s">
+        <v>586</v>
+      </c>
+      <c r="F221" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G221" t="s">
+        <v>587</v>
+      </c>
+      <c r="H221" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I221" t="s">
+        <v>93</v>
+      </c>
+      <c r="J221" t="s">
+        <v>94</v>
+      </c>
+      <c r="K221" t="s">
+        <v>199</v>
+      </c>
+      <c r="L221" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="222" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D222" t="s">
+        <v>588</v>
+      </c>
+      <c r="F222" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G222" t="s">
+        <v>589</v>
+      </c>
+      <c r="H222" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I222" t="s">
+        <v>93</v>
+      </c>
+      <c r="J222" t="s">
+        <v>94</v>
+      </c>
+      <c r="K222" t="s">
+        <v>199</v>
+      </c>
+      <c r="L222" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="223" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D223" t="s">
+        <v>590</v>
+      </c>
+      <c r="F223" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G223" t="s">
+        <v>591</v>
+      </c>
+      <c r="H223" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I223" t="s">
+        <v>93</v>
+      </c>
+      <c r="J223" t="s">
+        <v>94</v>
+      </c>
+      <c r="K223" t="s">
+        <v>199</v>
+      </c>
+      <c r="L223" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="224" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D224" t="s">
+        <v>592</v>
+      </c>
+      <c r="F224" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G224" t="s">
+        <v>593</v>
+      </c>
+      <c r="H224" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I224" t="s">
+        <v>93</v>
+      </c>
+      <c r="J224" t="s">
+        <v>94</v>
+      </c>
+      <c r="K224" t="s">
+        <v>199</v>
+      </c>
+      <c r="L224" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="225" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D225" t="s">
+        <v>594</v>
+      </c>
+      <c r="F225" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G225" t="s">
+        <v>595</v>
+      </c>
+      <c r="H225" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I225" t="s">
+        <v>93</v>
+      </c>
+      <c r="J225" t="s">
+        <v>94</v>
+      </c>
+      <c r="K225" t="s">
+        <v>199</v>
+      </c>
+      <c r="L225" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="226" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D226" t="s">
+        <v>596</v>
+      </c>
+      <c r="F226" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G226" t="s">
+        <v>596</v>
+      </c>
+      <c r="H226" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I226" t="s">
+        <v>93</v>
+      </c>
+      <c r="J226" t="s">
+        <v>94</v>
+      </c>
+      <c r="K226" t="s">
+        <v>283</v>
+      </c>
+      <c r="L226" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="227" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D227" t="s">
+        <v>597</v>
+      </c>
+      <c r="F227" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G227" t="s">
+        <v>597</v>
+      </c>
+      <c r="H227" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I227" t="s">
+        <v>93</v>
+      </c>
+      <c r="J227" t="s">
+        <v>94</v>
+      </c>
+      <c r="K227" t="s">
+        <v>283</v>
+      </c>
+      <c r="L227" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="228" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D228" t="s">
+        <v>598</v>
+      </c>
+      <c r="F228" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G228" t="s">
+        <v>283</v>
+      </c>
+      <c r="H228" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I228" t="s">
+        <v>93</v>
+      </c>
+      <c r="J228" t="s">
+        <v>94</v>
+      </c>
+      <c r="K228" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="229" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D229" t="s">
+        <v>599</v>
+      </c>
+      <c r="F229" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G229" t="s">
+        <v>600</v>
+      </c>
+      <c r="H229" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I229" t="s">
+        <v>93</v>
+      </c>
+      <c r="J229" t="s">
+        <v>94</v>
+      </c>
+      <c r="K229" t="s">
+        <v>283</v>
+      </c>
+      <c r="L229" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="230" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D230" t="s">
+        <v>601</v>
+      </c>
+      <c r="F230" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G230" s="30" t="s">
+        <v>605</v>
+      </c>
+      <c r="H230" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="I230" t="s">
+        <v>93</v>
+      </c>
+      <c r="J230" t="s">
+        <v>94</v>
+      </c>
+      <c r="K230" t="s">
+        <v>283</v>
+      </c>
+      <c r="L230" t="s">
+        <v>602</v>
+      </c>
+      <c r="M230" t="s">
+        <v>603</v>
+      </c>
+      <c r="N230" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="231" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D231" t="s">
+        <v>606</v>
+      </c>
+      <c r="F231" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G231" t="s">
+        <v>283</v>
+      </c>
+      <c r="H231" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I231" t="s">
+        <v>93</v>
+      </c>
+      <c r="J231" t="s">
+        <v>94</v>
+      </c>
+      <c r="K231" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="232" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D232" t="s">
+        <v>607</v>
+      </c>
+      <c r="F232" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G232" t="s">
+        <v>607</v>
+      </c>
+      <c r="H232" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I232" t="s">
+        <v>93</v>
+      </c>
+      <c r="J232" t="s">
+        <v>94</v>
+      </c>
+      <c r="K232" t="s">
+        <v>228</v>
+      </c>
+      <c r="L232" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="233" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D233" t="s">
+        <v>608</v>
+      </c>
+      <c r="F233" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G233" t="s">
+        <v>608</v>
+      </c>
+      <c r="H233" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I233" t="s">
+        <v>93</v>
+      </c>
+      <c r="J233" t="s">
+        <v>94</v>
+      </c>
+      <c r="K233" t="s">
+        <v>228</v>
+      </c>
+      <c r="L233" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="234" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D234" t="s">
+        <v>609</v>
+      </c>
+      <c r="F234" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G234" t="s">
+        <v>609</v>
+      </c>
+      <c r="H234" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I234" t="s">
+        <v>93</v>
+      </c>
+      <c r="J234" t="s">
+        <v>94</v>
+      </c>
+      <c r="K234" t="s">
+        <v>228</v>
+      </c>
+      <c r="L234" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="235" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D235" t="s">
+        <v>610</v>
+      </c>
+      <c r="F235" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G235" t="s">
+        <v>610</v>
+      </c>
+      <c r="H235" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I235" t="s">
+        <v>93</v>
+      </c>
+      <c r="J235" t="s">
+        <v>94</v>
+      </c>
+      <c r="K235" t="s">
+        <v>228</v>
+      </c>
+      <c r="L235" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="236" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D236" t="s">
+        <v>611</v>
+      </c>
+      <c r="F236" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G236" t="s">
+        <v>611</v>
+      </c>
+      <c r="H236" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I236" t="s">
+        <v>93</v>
+      </c>
+      <c r="J236" t="s">
+        <v>94</v>
+      </c>
+      <c r="K236" t="s">
+        <v>228</v>
+      </c>
+      <c r="L236" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="237" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D237" t="s">
+        <v>612</v>
+      </c>
+      <c r="F237" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G237" t="s">
+        <v>228</v>
+      </c>
+      <c r="H237" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I237" t="s">
+        <v>93</v>
+      </c>
+      <c r="J237" t="s">
+        <v>94</v>
+      </c>
+      <c r="K237" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="238" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D238" t="s">
+        <v>613</v>
+      </c>
+      <c r="F238" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G238" t="s">
+        <v>613</v>
+      </c>
+      <c r="H238" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I238" t="s">
+        <v>93</v>
+      </c>
+      <c r="J238" t="s">
+        <v>94</v>
+      </c>
+      <c r="K238" t="s">
+        <v>228</v>
+      </c>
+      <c r="L238" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="239" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D239" t="s">
+        <v>614</v>
+      </c>
+      <c r="F239" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G239" t="s">
+        <v>614</v>
+      </c>
+      <c r="H239" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I239" t="s">
+        <v>93</v>
+      </c>
+      <c r="J239" t="s">
+        <v>94</v>
+      </c>
+      <c r="K239" t="s">
+        <v>228</v>
+      </c>
+      <c r="L239" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="240" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D240" t="s">
+        <v>615</v>
+      </c>
+      <c r="F240" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G240" t="s">
+        <v>228</v>
+      </c>
+      <c r="H240" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I240" t="s">
+        <v>93</v>
+      </c>
+      <c r="J240" t="s">
+        <v>94</v>
+      </c>
+      <c r="K240" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="241" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D241" t="s">
+        <v>616</v>
+      </c>
+      <c r="F241" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G241" t="s">
+        <v>617</v>
+      </c>
+      <c r="H241" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I241" t="s">
+        <v>93</v>
+      </c>
+      <c r="J241" t="s">
+        <v>94</v>
+      </c>
+      <c r="K241" t="s">
+        <v>228</v>
+      </c>
+      <c r="L241" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="242" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D242" t="s">
+        <v>618</v>
+      </c>
+      <c r="F242" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="G242" t="s">
+        <v>617</v>
+      </c>
+      <c r="H242" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I242" t="s">
+        <v>93</v>
+      </c>
+      <c r="J242" t="s">
+        <v>94</v>
+      </c>
+      <c r="K242" t="s">
+        <v>228</v>
+      </c>
+      <c r="L242" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="243" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D243" t="s">
+        <v>619</v>
+      </c>
+      <c r="F243" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G243" t="s">
+        <v>227</v>
+      </c>
+      <c r="H243" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I243" t="s">
+        <v>93</v>
+      </c>
+      <c r="J243" t="s">
+        <v>94</v>
+      </c>
+      <c r="K243" t="s">
+        <v>228</v>
+      </c>
+      <c r="L243" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="244" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D244" t="s">
+        <v>620</v>
+      </c>
+      <c r="F244" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G244" t="s">
+        <v>228</v>
+      </c>
+      <c r="H244" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I244" t="s">
+        <v>93</v>
+      </c>
+      <c r="J244" t="s">
+        <v>94</v>
+      </c>
+      <c r="K244" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="245" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D245" t="s">
+        <v>621</v>
+      </c>
+      <c r="F245" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G245" t="s">
+        <v>622</v>
+      </c>
+      <c r="H245" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I245" t="s">
+        <v>93</v>
+      </c>
+      <c r="J245" t="s">
+        <v>94</v>
+      </c>
+      <c r="K245" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="246" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D246" t="s">
+        <v>623</v>
+      </c>
+      <c r="F246" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G246" t="s">
+        <v>622</v>
+      </c>
+      <c r="H246" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I246" t="s">
+        <v>93</v>
+      </c>
+      <c r="J246" t="s">
+        <v>94</v>
+      </c>
+      <c r="K246" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="247" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D247" t="s">
+        <v>624</v>
+      </c>
+      <c r="F247" s="30" t="s">
+        <v>298</v>
+      </c>
+      <c r="G247" t="s">
+        <v>622</v>
+      </c>
+      <c r="H247" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I247" t="s">
+        <v>93</v>
+      </c>
+      <c r="J247" t="s">
+        <v>94</v>
+      </c>
+      <c r="K247" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="248" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D248" t="s">
+        <v>625</v>
+      </c>
+      <c r="F248" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G248" t="s">
+        <v>627</v>
+      </c>
+      <c r="H248" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I248" t="s">
+        <v>93</v>
+      </c>
+      <c r="J248" t="s">
+        <v>94</v>
+      </c>
+      <c r="K248" t="s">
+        <v>626</v>
+      </c>
+      <c r="L248" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="249" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D249" t="s">
+        <v>628</v>
+      </c>
+      <c r="F249" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G249" t="s">
+        <v>630</v>
+      </c>
+      <c r="H249" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I249" t="s">
+        <v>93</v>
+      </c>
+      <c r="J249" t="s">
+        <v>94</v>
+      </c>
+      <c r="K249" t="s">
+        <v>629</v>
+      </c>
+      <c r="L249" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="250" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D250" t="s">
+        <v>631</v>
+      </c>
+      <c r="F250" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G250" t="s">
+        <v>629</v>
+      </c>
+      <c r="H250" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I250" t="s">
+        <v>93</v>
+      </c>
+      <c r="J250" t="s">
+        <v>94</v>
+      </c>
+      <c r="K250" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="251" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D251" t="s">
+        <v>632</v>
+      </c>
+      <c r="F251" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G251" t="s">
+        <v>633</v>
+      </c>
+      <c r="H251" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I251" t="s">
+        <v>93</v>
+      </c>
+      <c r="J251" t="s">
+        <v>94</v>
+      </c>
+      <c r="K251" t="s">
+        <v>272</v>
+      </c>
+      <c r="L251" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="252" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D252" t="s">
+        <v>634</v>
+      </c>
+      <c r="F252" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G252" t="s">
+        <v>272</v>
+      </c>
+      <c r="H252" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I252" t="s">
+        <v>93</v>
+      </c>
+      <c r="J252" t="s">
+        <v>94</v>
+      </c>
+      <c r="K252" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="253" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D253" t="s">
+        <v>635</v>
+      </c>
+      <c r="F253" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G253" t="s">
+        <v>635</v>
+      </c>
+      <c r="H253" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I253" t="s">
+        <v>93</v>
+      </c>
+      <c r="J253" t="s">
+        <v>94</v>
+      </c>
+      <c r="K253" t="s">
+        <v>272</v>
+      </c>
+      <c r="L253" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="254" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D254" t="s">
+        <v>636</v>
+      </c>
+      <c r="F254" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G254" t="s">
+        <v>636</v>
+      </c>
+      <c r="H254" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I254" t="s">
+        <v>93</v>
+      </c>
+      <c r="J254" t="s">
+        <v>94</v>
+      </c>
+      <c r="K254" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="255" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D255" t="s">
+        <v>637</v>
+      </c>
+      <c r="F255" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G255" t="s">
+        <v>638</v>
+      </c>
+      <c r="H255" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I255" t="s">
+        <v>93</v>
+      </c>
+      <c r="J255" t="s">
+        <v>94</v>
+      </c>
+      <c r="K255" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="256" spans="4:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="D256" t="s">
+        <v>639</v>
+      </c>
+      <c r="F256" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G256" t="s">
+        <v>638</v>
+      </c>
+      <c r="H256" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I256" t="s">
+        <v>93</v>
+      </c>
+      <c r="J256" t="s">
+        <v>94</v>
+      </c>
+      <c r="K256" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="257" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D257" t="s">
+        <v>640</v>
+      </c>
+      <c r="F257" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G257" t="s">
+        <v>249</v>
+      </c>
+      <c r="H257" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I257" t="s">
+        <v>93</v>
+      </c>
+      <c r="J257" t="s">
+        <v>94</v>
+      </c>
+      <c r="K257" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="258" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D258" t="s">
+        <v>641</v>
+      </c>
+      <c r="F258" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G258" t="s">
+        <v>250</v>
+      </c>
+      <c r="H258" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I258" t="s">
+        <v>93</v>
+      </c>
+      <c r="J258" t="s">
+        <v>94</v>
+      </c>
+      <c r="K258" t="s">
+        <v>249</v>
+      </c>
+      <c r="L258" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="259" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D259" t="s">
+        <v>642</v>
+      </c>
+      <c r="F259" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G259" t="s">
+        <v>643</v>
+      </c>
+      <c r="H259" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I259" t="s">
+        <v>93</v>
+      </c>
+      <c r="J259" t="s">
+        <v>94</v>
+      </c>
+      <c r="K259" t="s">
+        <v>249</v>
+      </c>
+      <c r="L259" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="260" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D260" t="s">
+        <v>644</v>
+      </c>
+      <c r="F260" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G260" t="s">
+        <v>249</v>
+      </c>
+      <c r="H260" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I260" t="s">
+        <v>93</v>
+      </c>
+      <c r="J260" t="s">
+        <v>94</v>
+      </c>
+      <c r="K260" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="261" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D261" t="s">
+        <v>645</v>
+      </c>
+      <c r="F261" s="30" t="s">
+        <v>298</v>
+      </c>
+      <c r="G261" t="s">
+        <v>250</v>
+      </c>
+      <c r="H261" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I261" t="s">
+        <v>93</v>
+      </c>
+      <c r="J261" t="s">
+        <v>94</v>
+      </c>
+      <c r="K261" t="s">
+        <v>249</v>
+      </c>
+      <c r="L261" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="262" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D262" t="s">
+        <v>646</v>
+      </c>
+      <c r="F262" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G262" t="s">
+        <v>94</v>
+      </c>
+      <c r="H262" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="I262" t="s">
+        <v>93</v>
+      </c>
+      <c r="J262" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="263" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D263" t="s">
+        <v>647</v>
+      </c>
+      <c r="F263" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="G263" t="s">
+        <v>224</v>
+      </c>
+      <c r="H263" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I263" t="s">
+        <v>93</v>
+      </c>
+      <c r="J263" t="s">
+        <v>102</v>
+      </c>
+      <c r="K263" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="264" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D264" t="s">
+        <v>648</v>
+      </c>
+      <c r="F264" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G264" t="s">
+        <v>648</v>
+      </c>
+      <c r="H264" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I264" t="s">
+        <v>93</v>
+      </c>
+      <c r="J264" t="s">
+        <v>102</v>
+      </c>
+      <c r="K264" t="s">
+        <v>224</v>
+      </c>
+      <c r="L264" t="s">
+        <v>649</v>
+      </c>
+      <c r="M264" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="265" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D265" t="s">
+        <v>650</v>
+      </c>
+      <c r="F265" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G265" t="s">
+        <v>650</v>
+      </c>
+      <c r="H265" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I265" t="s">
+        <v>93</v>
+      </c>
+      <c r="J265" t="s">
+        <v>102</v>
+      </c>
+      <c r="K265" t="s">
+        <v>224</v>
+      </c>
+      <c r="L265" t="s">
+        <v>651</v>
+      </c>
+      <c r="M265" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="266" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D266" t="s">
+        <v>653</v>
+      </c>
+      <c r="F266" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G266" t="s">
+        <v>653</v>
+      </c>
+      <c r="H266" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I266" t="s">
+        <v>93</v>
+      </c>
+      <c r="J266" t="s">
+        <v>102</v>
+      </c>
+      <c r="K266" t="s">
+        <v>224</v>
+      </c>
+      <c r="L266" t="s">
+        <v>654</v>
+      </c>
+      <c r="M266" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="267" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D267" t="s">
+        <v>655</v>
+      </c>
+      <c r="F267" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G267" t="s">
+        <v>655</v>
+      </c>
+      <c r="H267" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I267" t="s">
+        <v>93</v>
+      </c>
+      <c r="J267" t="s">
+        <v>656</v>
+      </c>
+      <c r="K267" t="s">
+        <v>224</v>
+      </c>
+      <c r="L267" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="268" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D268" t="s">
+        <v>657</v>
+      </c>
+      <c r="F268" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G268" t="s">
+        <v>144</v>
+      </c>
+      <c r="H268" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I268" t="s">
+        <v>93</v>
+      </c>
+      <c r="J268" t="s">
+        <v>102</v>
+      </c>
+      <c r="K268" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="269" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D269" t="s">
+        <v>658</v>
+      </c>
+      <c r="F269" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G269" t="s">
+        <v>661</v>
+      </c>
+      <c r="H269" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="I269" t="s">
+        <v>93</v>
+      </c>
+      <c r="J269" t="s">
+        <v>102</v>
+      </c>
+      <c r="K269" t="s">
+        <v>144</v>
+      </c>
+      <c r="L269" t="s">
+        <v>659</v>
+      </c>
+      <c r="M269" t="s">
+        <v>658</v>
+      </c>
+      <c r="N269" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="270" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D270" t="s">
+        <v>662</v>
+      </c>
+      <c r="F270" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G270" t="s">
+        <v>144</v>
+      </c>
+      <c r="H270" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I270" t="s">
+        <v>93</v>
+      </c>
+      <c r="J270" t="s">
+        <v>102</v>
+      </c>
+      <c r="K270" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="271" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D271" t="s">
+        <v>663</v>
+      </c>
+      <c r="F271" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G271" t="s">
+        <v>665</v>
+      </c>
+      <c r="H271" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I271" t="s">
+        <v>93</v>
+      </c>
+      <c r="J271" t="s">
+        <v>102</v>
+      </c>
+      <c r="K271" t="s">
+        <v>144</v>
+      </c>
+      <c r="L271" t="s">
+        <v>664</v>
+      </c>
+      <c r="M271" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="272" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D272" t="s">
+        <v>666</v>
+      </c>
+      <c r="F272" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G272" t="s">
+        <v>666</v>
+      </c>
+      <c r="H272" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I272" t="s">
+        <v>93</v>
+      </c>
+      <c r="J272" t="s">
+        <v>102</v>
+      </c>
+      <c r="K272" t="s">
+        <v>144</v>
+      </c>
+      <c r="L272" t="s">
+        <v>659</v>
+      </c>
+      <c r="M272" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="273" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D273" t="s">
+        <v>667</v>
+      </c>
+      <c r="F273" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="G273" t="s">
+        <v>144</v>
+      </c>
+      <c r="H273" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I273" t="s">
+        <v>93</v>
+      </c>
+      <c r="J273" t="s">
+        <v>102</v>
+      </c>
+      <c r="K273" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="274" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D274" t="s">
+        <v>668</v>
+      </c>
+      <c r="F274" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G274" t="s">
+        <v>668</v>
+      </c>
+      <c r="H274" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I274" t="s">
+        <v>93</v>
+      </c>
+      <c r="J274" t="s">
+        <v>102</v>
+      </c>
+      <c r="K274" t="s">
+        <v>144</v>
+      </c>
+      <c r="L274" t="s">
+        <v>669</v>
+      </c>
+      <c r="M274" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="275" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D275" t="s">
+        <v>670</v>
+      </c>
+      <c r="F275" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G275" s="30" t="s">
+        <v>673</v>
+      </c>
+      <c r="H275" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="I275" t="s">
+        <v>93</v>
+      </c>
+      <c r="J275" t="s">
+        <v>102</v>
+      </c>
+      <c r="K275" t="s">
+        <v>144</v>
+      </c>
+      <c r="L275" t="s">
+        <v>269</v>
+      </c>
+      <c r="M275" t="s">
+        <v>671</v>
+      </c>
+      <c r="N275" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="276" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D276" t="s">
+        <v>674</v>
+      </c>
+      <c r="F276" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G276" t="s">
+        <v>666</v>
+      </c>
+      <c r="H276" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I276" t="s">
+        <v>93</v>
+      </c>
+      <c r="J276" t="s">
+        <v>102</v>
+      </c>
+      <c r="K276" t="s">
+        <v>144</v>
+      </c>
+      <c r="L276" t="s">
+        <v>659</v>
+      </c>
+      <c r="M276" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="277" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D277" t="s">
+        <v>675</v>
+      </c>
+      <c r="F277" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G277" t="s">
+        <v>675</v>
+      </c>
+      <c r="H277" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I277" t="s">
+        <v>93</v>
+      </c>
+      <c r="J277" t="s">
+        <v>102</v>
+      </c>
+      <c r="K277" t="s">
+        <v>144</v>
+      </c>
+      <c r="L277" t="s">
+        <v>659</v>
+      </c>
+      <c r="M277" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="278" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D278" t="s">
+        <v>676</v>
+      </c>
+      <c r="F278" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G278" t="s">
+        <v>676</v>
+      </c>
+      <c r="H278" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I278" t="s">
+        <v>93</v>
+      </c>
+      <c r="J278" t="s">
+        <v>102</v>
+      </c>
+      <c r="K278" t="s">
+        <v>231</v>
+      </c>
+      <c r="L278" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="279" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D279" t="s">
+        <v>677</v>
+      </c>
+      <c r="F279" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G279" s="30" t="s">
+        <v>680</v>
+      </c>
+      <c r="H279" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="I279" t="s">
+        <v>93</v>
+      </c>
+      <c r="J279" t="s">
+        <v>102</v>
+      </c>
+      <c r="K279" t="s">
+        <v>231</v>
+      </c>
+      <c r="L279" t="s">
+        <v>678</v>
+      </c>
+      <c r="M279" t="s">
+        <v>677</v>
+      </c>
+      <c r="N279" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="280" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D280" t="s">
+        <v>681</v>
+      </c>
+      <c r="F280" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G280" t="s">
+        <v>681</v>
+      </c>
+      <c r="H280" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I280" t="s">
+        <v>93</v>
+      </c>
+      <c r="J280" t="s">
+        <v>102</v>
+      </c>
+      <c r="K280" t="s">
+        <v>231</v>
+      </c>
+      <c r="L280" t="s">
+        <v>676</v>
+      </c>
+      <c r="M280" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="281" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D281" t="s">
+        <v>682</v>
+      </c>
+      <c r="F281" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G281" t="s">
+        <v>682</v>
+      </c>
+      <c r="H281" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I281" t="s">
+        <v>93</v>
+      </c>
+      <c r="J281" t="s">
+        <v>102</v>
+      </c>
+      <c r="K281" t="s">
+        <v>231</v>
+      </c>
+      <c r="L281" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="282" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D282" t="s">
+        <v>683</v>
+      </c>
+      <c r="F282" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G282" t="s">
+        <v>231</v>
+      </c>
+      <c r="H282" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I282" t="s">
+        <v>93</v>
+      </c>
+      <c r="J282" t="s">
+        <v>102</v>
+      </c>
+      <c r="K282" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="283" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D283" t="s">
+        <v>684</v>
+      </c>
+      <c r="F283" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="G283" t="s">
+        <v>231</v>
+      </c>
+      <c r="H283" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I283" t="s">
+        <v>93</v>
+      </c>
+      <c r="J283" t="s">
+        <v>102</v>
+      </c>
+      <c r="K283" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="284" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D284" t="s">
+        <v>685</v>
+      </c>
+      <c r="F284" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G284" s="30" t="s">
+        <v>686</v>
+      </c>
+      <c r="H284" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="I284" t="s">
+        <v>93</v>
+      </c>
+      <c r="J284" t="s">
+        <v>102</v>
+      </c>
+      <c r="K284" t="s">
+        <v>268</v>
+      </c>
+      <c r="L284" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="M284" t="s">
+        <v>688</v>
+      </c>
+      <c r="N284" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="285" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D285" t="s">
+        <v>689</v>
+      </c>
+      <c r="F285" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G285" s="30" t="s">
+        <v>690</v>
+      </c>
+      <c r="H285" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="I285" t="s">
+        <v>93</v>
+      </c>
+      <c r="J285" t="s">
+        <v>102</v>
+      </c>
+      <c r="K285" t="s">
+        <v>268</v>
+      </c>
+      <c r="L285" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="M285" s="30" t="s">
+        <v>222</v>
+      </c>
+      <c r="N285" s="30" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="286" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D286" t="s">
+        <v>692</v>
+      </c>
+      <c r="F286" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G286" s="30" t="s">
+        <v>693</v>
+      </c>
+      <c r="H286" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="I286" t="s">
+        <v>93</v>
+      </c>
+      <c r="J286" t="s">
+        <v>102</v>
+      </c>
+      <c r="K286" t="s">
+        <v>268</v>
+      </c>
+      <c r="L286" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="M286" s="30" t="s">
+        <v>694</v>
+      </c>
+      <c r="N286" s="30" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="287" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D287" t="s">
+        <v>696</v>
+      </c>
+      <c r="F287" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G287" s="30" t="s">
+        <v>697</v>
+      </c>
+      <c r="H287" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="I287" t="s">
+        <v>93</v>
+      </c>
+      <c r="J287" t="s">
+        <v>102</v>
+      </c>
+      <c r="K287" t="s">
+        <v>268</v>
+      </c>
+      <c r="L287" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="M287" s="30" t="s">
+        <v>698</v>
+      </c>
+      <c r="N287" s="30" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="288" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D288" t="s">
+        <v>700</v>
+      </c>
+      <c r="F288" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G288" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="H288" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I288" t="s">
+        <v>93</v>
+      </c>
+      <c r="J288" t="s">
+        <v>102</v>
+      </c>
+      <c r="K288" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="289" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D289" t="s">
+        <v>701</v>
+      </c>
+      <c r="F289" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="G289" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="H289" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I289" t="s">
+        <v>93</v>
+      </c>
+      <c r="J289" t="s">
+        <v>102</v>
+      </c>
+      <c r="K289" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="290" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D290" t="s">
+        <v>686</v>
+      </c>
+      <c r="F290" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G290" s="30" t="s">
+        <v>686</v>
+      </c>
+      <c r="H290" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="I290" t="s">
+        <v>93</v>
+      </c>
+      <c r="J290" t="s">
+        <v>102</v>
+      </c>
+      <c r="K290" t="s">
+        <v>268</v>
+      </c>
+      <c r="L290" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="M290" t="s">
+        <v>688</v>
+      </c>
+      <c r="N290" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="291" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D291" t="s">
+        <v>702</v>
+      </c>
+      <c r="F291" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G291" t="s">
+        <v>102</v>
+      </c>
+      <c r="H291" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="I291" t="s">
+        <v>93</v>
+      </c>
+      <c r="J291" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="292" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D292" t="s">
+        <v>703</v>
+      </c>
+      <c r="F292" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G292" t="s">
+        <v>709</v>
+      </c>
+      <c r="H292" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="I292" t="s">
+        <v>704</v>
+      </c>
+      <c r="J292" t="s">
+        <v>705</v>
+      </c>
+      <c r="K292" t="s">
+        <v>706</v>
+      </c>
+      <c r="L292" t="s">
+        <v>707</v>
+      </c>
+      <c r="M292" t="s">
+        <v>708</v>
+      </c>
+      <c r="N292" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="293" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D293" t="s">
+        <v>711</v>
+      </c>
+      <c r="F293" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G293" t="s">
+        <v>264</v>
+      </c>
+      <c r="H293" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="I293" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="294" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D294" t="s">
+        <v>712</v>
+      </c>
+      <c r="F294" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G294" t="s">
+        <v>714</v>
+      </c>
+      <c r="H294" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I294" t="s">
+        <v>264</v>
+      </c>
+      <c r="J294" t="s">
+        <v>265</v>
+      </c>
+      <c r="K294" t="s">
+        <v>715</v>
+      </c>
+      <c r="L294" t="s">
+        <v>713</v>
+      </c>
+      <c r="M294" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="295" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D295" t="s">
+        <v>716</v>
+      </c>
+      <c r="F295" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G295" t="s">
+        <v>264</v>
+      </c>
+      <c r="H295" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="I295" t="s">
+        <v>264</v>
+      </c>
+      <c r="J295"/>
+    </row>
+    <row r="296" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D296" t="s">
+        <v>717</v>
+      </c>
+      <c r="F296" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G296" t="s">
+        <v>717</v>
+      </c>
+      <c r="H296" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I296" t="s">
+        <v>264</v>
+      </c>
+      <c r="J296" t="s">
+        <v>265</v>
+      </c>
+      <c r="K296" t="s">
+        <v>719</v>
+      </c>
+      <c r="L296" t="s">
+        <v>718</v>
+      </c>
+      <c r="M296" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="297" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D297" t="s">
+        <v>720</v>
+      </c>
+      <c r="F297" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G297" t="s">
+        <v>722</v>
+      </c>
+      <c r="H297" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I297" t="s">
+        <v>264</v>
+      </c>
+      <c r="J297" t="s">
+        <v>723</v>
+      </c>
+      <c r="K297" t="s">
+        <v>724</v>
+      </c>
+      <c r="L297" t="s">
+        <v>721</v>
+      </c>
+      <c r="M297" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="298" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D298" t="s">
+        <v>725</v>
+      </c>
+      <c r="F298" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G298" t="s">
+        <v>729</v>
+      </c>
+      <c r="H298" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="I298" t="s">
+        <v>243</v>
+      </c>
+      <c r="J298" t="s">
+        <v>307</v>
+      </c>
+      <c r="K298" t="s">
+        <v>726</v>
+      </c>
+      <c r="L298" t="s">
+        <v>727</v>
+      </c>
+      <c r="M298" t="s">
+        <v>725</v>
+      </c>
+      <c r="N298" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="299" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D299" t="s">
+        <v>730</v>
+      </c>
+      <c r="F299" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="G299" t="s">
+        <v>307</v>
+      </c>
+      <c r="H299" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="I299" t="s">
+        <v>243</v>
+      </c>
+      <c r="J299" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="300" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D300" t="s">
+        <v>731</v>
+      </c>
+      <c r="F300" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G300" t="s">
+        <v>735</v>
+      </c>
+      <c r="H300" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="I300" t="s">
+        <v>243</v>
+      </c>
+      <c r="J300" t="s">
+        <v>307</v>
+      </c>
+      <c r="K300" t="s">
+        <v>732</v>
+      </c>
+      <c r="L300" t="s">
+        <v>733</v>
+      </c>
+      <c r="M300" t="s">
+        <v>731</v>
+      </c>
+      <c r="N300" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="301" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D301" t="s">
+        <v>736</v>
+      </c>
+      <c r="F301" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G301" t="s">
+        <v>307</v>
+      </c>
+      <c r="H301" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="I301" t="s">
+        <v>243</v>
+      </c>
+      <c r="J301" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="302" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D302" t="s">
+        <v>737</v>
+      </c>
+      <c r="F302" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G302" t="s">
+        <v>737</v>
+      </c>
+      <c r="H302" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I302" t="s">
+        <v>243</v>
+      </c>
+      <c r="J302" t="s">
+        <v>738</v>
+      </c>
+      <c r="K302" t="s">
+        <v>740</v>
+      </c>
+      <c r="L302" t="s">
+        <v>739</v>
+      </c>
+      <c r="M302" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="303" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D303" t="s">
+        <v>741</v>
+      </c>
+      <c r="F303" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G303" t="s">
+        <v>741</v>
+      </c>
+      <c r="H303" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I303" t="s">
+        <v>243</v>
+      </c>
+      <c r="J303" t="s">
+        <v>244</v>
+      </c>
+      <c r="K303" t="s">
+        <v>742</v>
+      </c>
+      <c r="L303" t="s">
+        <v>743</v>
+      </c>
+      <c r="M303" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="304" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D304" t="s">
+        <v>744</v>
+      </c>
+      <c r="F304" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G304" t="s">
+        <v>744</v>
+      </c>
+      <c r="H304" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I304" t="s">
+        <v>243</v>
+      </c>
+      <c r="J304" t="s">
+        <v>244</v>
+      </c>
+      <c r="K304" t="s">
+        <v>742</v>
+      </c>
+      <c r="L304" t="s">
+        <v>743</v>
+      </c>
+      <c r="M304" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="305" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D305" t="s">
+        <v>745</v>
+      </c>
+      <c r="F305" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G305" t="s">
+        <v>745</v>
+      </c>
+      <c r="H305" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I305" t="s">
+        <v>243</v>
+      </c>
+      <c r="J305" t="s">
+        <v>244</v>
+      </c>
+      <c r="K305" t="s">
+        <v>740</v>
+      </c>
+      <c r="L305" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="306" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D306" t="s">
+        <v>746</v>
+      </c>
+      <c r="F306" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G306" t="s">
+        <v>747</v>
+      </c>
+      <c r="H306" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I306" t="s">
+        <v>243</v>
+      </c>
+      <c r="J306" t="s">
+        <v>244</v>
+      </c>
+      <c r="K306" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="307" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D307" t="s">
+        <v>748</v>
+      </c>
+      <c r="F307" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G307" t="s">
+        <v>748</v>
+      </c>
+      <c r="H307" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="I307" t="s">
+        <v>243</v>
+      </c>
+      <c r="J307" t="s">
+        <v>244</v>
+      </c>
+      <c r="K307" t="s">
+        <v>752</v>
+      </c>
+      <c r="L307" t="s">
+        <v>749</v>
+      </c>
+      <c r="M307" t="s">
+        <v>750</v>
+      </c>
+      <c r="N307" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="308" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D308" t="s">
+        <v>753</v>
+      </c>
+      <c r="F308" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G308" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H308" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="I308" t="s">
+        <v>243</v>
+      </c>
+      <c r="J308" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="309" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D309" t="s">
+        <v>754</v>
+      </c>
+      <c r="F309" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G309" t="s">
+        <v>754</v>
+      </c>
+      <c r="H309" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I309" t="s">
+        <v>243</v>
+      </c>
+      <c r="J309" t="s">
+        <v>244</v>
+      </c>
+      <c r="K309" t="s">
+        <v>755</v>
+      </c>
+      <c r="L309" t="s">
+        <v>296</v>
+      </c>
+      <c r="M309" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="310" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D310" t="s">
+        <v>756</v>
+      </c>
+      <c r="F310" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G310" t="s">
+        <v>296</v>
+      </c>
+      <c r="H310" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I310" t="s">
+        <v>243</v>
+      </c>
+      <c r="J310" t="s">
+        <v>244</v>
+      </c>
+      <c r="K310" t="s">
+        <v>755</v>
+      </c>
+      <c r="L310" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="311" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D311" t="s">
+        <v>757</v>
+      </c>
+      <c r="F311" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G311" t="s">
+        <v>244</v>
+      </c>
+      <c r="H311" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="I311" t="s">
+        <v>243</v>
+      </c>
+      <c r="J311" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="312" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D312" t="s">
+        <v>758</v>
+      </c>
+      <c r="F312" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G312" t="s">
+        <v>758</v>
+      </c>
+      <c r="H312" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I312" t="s">
+        <v>759</v>
+      </c>
+      <c r="J312" t="s">
+        <v>760</v>
+      </c>
+      <c r="K312" t="s">
+        <v>761</v>
+      </c>
+      <c r="L312" t="s">
+        <v>762</v>
+      </c>
+      <c r="M312" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="313" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D313" t="s">
+        <v>759</v>
+      </c>
+      <c r="F313" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G313" t="s">
+        <v>759</v>
+      </c>
+      <c r="H313" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="I313" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="314" spans="4:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="D314" t="s">
+        <v>763</v>
+      </c>
+      <c r="F314" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G314" t="s">
+        <v>763</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made minor changes to app after meeting 11/22
</commit_message>
<xml_diff>
--- a/Data/new_crosswalk.xlsx
+++ b/Data/new_crosswalk.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\ZoopSynth\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E083BF34-3CAF-4F20-A544-306C1BA4187F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LCD" sheetId="4" r:id="rId1"/>
@@ -1577,9 +1578,6 @@
     <t>YBFMP</t>
   </si>
   <si>
-    <t>Mixed</t>
-  </si>
-  <si>
     <t>OTHCYCADPUMP</t>
   </si>
   <si>
@@ -2472,12 +2470,15 @@
   </si>
   <si>
     <t>clam other</t>
+  </si>
+  <si>
+    <t>Undifferentiated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -2733,9 +2734,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal_20mm" xfId="2"/>
-    <cellStyle name="Normal_Species Lookup" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal_20mm" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal_Species Lookup" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3012,7 +3013,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
@@ -3913,12 +3914,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P258" sqref="P258"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3949,34 +3950,34 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
+        <v>768</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>769</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="C1" s="31" t="s">
         <v>770</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="D1" s="31" t="s">
         <v>771</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="E1" s="31" t="s">
         <v>772</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="F1" s="31" t="s">
         <v>773</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="G1" s="31" t="s">
         <v>774</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="H1" s="31" t="s">
         <v>775</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="I1" s="31" t="s">
         <v>776</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="J1" s="31" t="s">
         <v>777</v>
-      </c>
-      <c r="J1" s="31" t="s">
-        <v>778</v>
       </c>
       <c r="K1" s="31" t="s">
         <v>488</v>
@@ -4413,10 +4414,10 @@
         <v>129</v>
       </c>
       <c r="I8" s="33" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="J8" s="33" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="K8" s="31" t="s">
         <v>400</v>
@@ -4463,10 +4464,10 @@
       <c r="G9" s="32"/>
       <c r="H9" s="31"/>
       <c r="I9" s="33" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="J9" s="33" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="K9" s="31"/>
       <c r="L9" s="31" t="s">
@@ -5649,10 +5650,10 @@
         <v>107</v>
       </c>
       <c r="I28" s="33" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="J28" s="33" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="K28" s="31" t="s">
         <v>376</v>
@@ -5751,7 +5752,7 @@
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
@@ -5761,10 +5762,10 @@
       <c r="G30" s="32"/>
       <c r="H30" s="31"/>
       <c r="I30" s="33" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="J30" s="33" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="K30" s="31"/>
       <c r="L30" s="31" t="s">
@@ -5828,7 +5829,7 @@
         <v>386</v>
       </c>
       <c r="L31" s="31" t="s">
-        <v>489</v>
+        <v>787</v>
       </c>
       <c r="M31" s="31" t="s">
         <v>133</v>
@@ -7733,10 +7734,10 @@
         <v>141</v>
       </c>
       <c r="I64" s="33" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="J64" s="33" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="K64" s="31"/>
       <c r="L64" s="31" t="s">
@@ -8649,7 +8650,7 @@
       <c r="A80" s="34"/>
       <c r="B80" s="34"/>
       <c r="C80" s="34" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D80" s="31"/>
       <c r="E80" s="31" t="s">
@@ -8715,11 +8716,11 @@
       <c r="C81" s="31"/>
       <c r="D81" s="38"/>
       <c r="E81" s="38" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="F81" s="38"/>
       <c r="G81" s="38" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="H81" s="31" t="s">
         <v>222</v>
@@ -9771,11 +9772,11 @@
       <c r="C103" s="31"/>
       <c r="D103" s="38"/>
       <c r="E103" s="38" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="F103" s="38"/>
       <c r="G103" s="38" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="H103" s="31"/>
       <c r="I103" s="31" t="s">
@@ -9875,7 +9876,7 @@
       <c r="A105" s="34"/>
       <c r="B105" s="34"/>
       <c r="C105" s="34" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="D105" s="38"/>
       <c r="E105" s="38" t="s">
@@ -10177,7 +10178,7 @@
       <c r="A111" s="34"/>
       <c r="B111" s="34"/>
       <c r="C111" s="34" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D111" s="38"/>
       <c r="E111" s="38" t="s">
@@ -10645,7 +10646,7 @@
         <v>242</v>
       </c>
       <c r="Q120" s="31" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="R120" s="31" t="s">
         <v>292</v>
@@ -10713,11 +10714,11 @@
       <c r="C122" s="31"/>
       <c r="D122" s="38"/>
       <c r="E122" s="38" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="F122" s="38"/>
       <c r="G122" s="38" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="H122" s="31"/>
       <c r="I122" s="31" t="s">
@@ -10807,11 +10808,11 @@
       <c r="C124" s="31"/>
       <c r="D124" s="38"/>
       <c r="E124" s="38" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="F124" s="38"/>
       <c r="G124" s="38" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="H124" s="31"/>
       <c r="I124" s="31" t="s">
@@ -10907,10 +10908,10 @@
       <c r="G126" s="38"/>
       <c r="H126" s="31"/>
       <c r="I126" s="31" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="J126" s="31" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="K126" s="31"/>
       <c r="L126" s="31" t="s">
@@ -10963,7 +10964,7 @@
         <v>207</v>
       </c>
       <c r="M127" s="31" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="N127" s="31" t="s">
         <v>84</v>
@@ -10975,7 +10976,7 @@
         <v>289</v>
       </c>
       <c r="Q127" s="31" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="R127" s="31"/>
       <c r="S127" s="31"/>
@@ -11477,11 +11478,11 @@
       <c r="C138" s="31"/>
       <c r="D138" s="38"/>
       <c r="E138" s="38" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="F138" s="38"/>
       <c r="G138" s="38" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="H138" s="31"/>
       <c r="I138" s="31" t="s">
@@ -11557,7 +11558,7 @@
         <v>242</v>
       </c>
       <c r="Q139" s="31" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="R139" s="31" t="s">
         <v>314</v>
@@ -12497,7 +12498,7 @@
         <v>207</v>
       </c>
       <c r="M159" s="31" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="N159" s="31" t="s">
         <v>87</v>
@@ -12515,7 +12516,7 @@
         <v>193</v>
       </c>
       <c r="S159" s="31" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="T159" s="31" t="s">
         <v>472</v>
@@ -12647,7 +12648,7 @@
         <v>208</v>
       </c>
       <c r="M162" s="31" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="N162" s="31" t="s">
         <v>87</v>
@@ -12665,7 +12666,7 @@
         <v>193</v>
       </c>
       <c r="S162" s="31" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="T162" s="31" t="s">
         <v>472</v>
@@ -12847,7 +12848,7 @@
         <v>207</v>
       </c>
       <c r="M166" s="31" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="N166" s="31" t="s">
         <v>87</v>
@@ -12865,7 +12866,7 @@
         <v>193</v>
       </c>
       <c r="S166" s="31" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="T166" s="31" t="s">
         <v>472</v>
@@ -12997,7 +12998,7 @@
         <v>207</v>
       </c>
       <c r="M169" s="31" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="N169" s="31" t="s">
         <v>87</v>
@@ -13018,7 +13019,7 @@
         <v>462</v>
       </c>
       <c r="T169" s="31" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="U169" s="31"/>
       <c r="V169" s="31"/>
@@ -13235,11 +13236,11 @@
       <c r="C174" s="31"/>
       <c r="D174" s="38"/>
       <c r="E174" s="38" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F174" s="38"/>
       <c r="G174" s="38" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H174" s="31"/>
       <c r="I174" s="31"/>
@@ -13249,7 +13250,7 @@
         <v>207</v>
       </c>
       <c r="M174" s="35" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="N174" s="31" t="s">
         <v>87</v>
@@ -13264,13 +13265,13 @@
         <v>223</v>
       </c>
       <c r="R174" s="31" t="s">
+        <v>494</v>
+      </c>
+      <c r="S174" s="31" t="s">
         <v>495</v>
       </c>
-      <c r="S174" s="31" t="s">
-        <v>496</v>
-      </c>
       <c r="T174" s="31" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="U174" s="31">
         <v>1954</v>
@@ -13289,25 +13290,25 @@
       <c r="C175" s="31"/>
       <c r="D175" s="38"/>
       <c r="E175" s="38" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F175" s="38"/>
       <c r="G175" s="38" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H175" s="31"/>
       <c r="I175" s="33" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J175" s="33" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="K175" s="31"/>
       <c r="L175" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M175" s="35" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="N175" s="31" t="s">
         <v>87</v>
@@ -13325,10 +13326,10 @@
         <v>272</v>
       </c>
       <c r="S175" s="31" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="T175" s="31" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="U175" s="31"/>
       <c r="V175" s="31"/>
@@ -13345,25 +13346,25 @@
       <c r="C176" s="31"/>
       <c r="D176" s="38"/>
       <c r="E176" s="38" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F176" s="38"/>
       <c r="G176" s="38" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="H176" s="31"/>
       <c r="I176" s="33" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J176" s="33" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="K176" s="31"/>
       <c r="L176" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M176" s="35" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="N176" s="31" t="s">
         <v>87</v>
@@ -13381,10 +13382,10 @@
         <v>272</v>
       </c>
       <c r="S176" s="31" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="T176" s="31" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="U176" s="31"/>
       <c r="V176" s="31"/>
@@ -13401,25 +13402,25 @@
       <c r="C177" s="31"/>
       <c r="D177" s="38"/>
       <c r="E177" s="38" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F177" s="38"/>
       <c r="G177" s="38" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H177" s="31"/>
       <c r="I177" s="33" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J177" s="33" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="K177" s="31"/>
       <c r="L177" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M177" s="35" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="N177" s="31" t="s">
         <v>87</v>
@@ -13437,10 +13438,10 @@
         <v>272</v>
       </c>
       <c r="S177" s="31" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="T177" s="31" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="U177" s="31">
         <v>1973</v>
@@ -13459,11 +13460,11 @@
       <c r="C178" s="31"/>
       <c r="D178" s="38"/>
       <c r="E178" s="38" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F178" s="38"/>
       <c r="G178" s="38" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H178" s="31"/>
       <c r="I178" s="31"/>
@@ -13473,7 +13474,7 @@
         <v>207</v>
       </c>
       <c r="M178" s="35" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="N178" s="31" t="s">
         <v>87</v>
@@ -13494,7 +13495,7 @@
         <v>222</v>
       </c>
       <c r="T178" s="31" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="U178" s="31">
         <v>1983</v>
@@ -13517,17 +13518,17 @@
       <c r="G179" s="38"/>
       <c r="H179" s="31"/>
       <c r="I179" s="33" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="J179" s="33" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K179" s="31"/>
       <c r="L179" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M179" s="33" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="N179" s="31" t="s">
         <v>86</v>
@@ -13542,10 +13543,10 @@
         <v>309</v>
       </c>
       <c r="R179" s="31" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="S179" s="31" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="T179" s="31"/>
       <c r="U179" s="31"/>
@@ -13611,17 +13612,17 @@
       <c r="G181" s="31"/>
       <c r="H181" s="31"/>
       <c r="I181" s="33" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="J181" s="33" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="K181" s="31"/>
       <c r="L181" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M181" s="33" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="N181" s="31" t="s">
         <v>87</v>
@@ -13633,16 +13634,16 @@
         <v>278</v>
       </c>
       <c r="Q181" s="31" t="s">
+        <v>750</v>
+      </c>
+      <c r="R181" s="31" t="s">
         <v>751</v>
       </c>
-      <c r="R181" s="31" t="s">
+      <c r="S181" s="31" t="s">
         <v>752</v>
       </c>
-      <c r="S181" s="31" t="s">
+      <c r="T181" s="31" t="s">
         <v>753</v>
-      </c>
-      <c r="T181" s="31" t="s">
-        <v>754</v>
       </c>
       <c r="U181" s="31"/>
       <c r="V181" s="31"/>
@@ -13713,17 +13714,17 @@
       <c r="G183" s="31"/>
       <c r="H183" s="31"/>
       <c r="I183" s="33" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="J183" s="33" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="K183" s="31"/>
       <c r="L183" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M183" s="33" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="N183" s="31" t="s">
         <v>86</v>
@@ -13741,7 +13742,7 @@
         <v>193</v>
       </c>
       <c r="S183" s="33" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="T183" s="31"/>
       <c r="U183" s="31"/>
@@ -13813,10 +13814,10 @@
       <c r="G185" s="31"/>
       <c r="H185" s="31"/>
       <c r="I185" s="33" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="J185" s="33" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K185" s="31"/>
       <c r="L185" s="31" t="s">
@@ -13857,10 +13858,10 @@
       <c r="G186" s="31"/>
       <c r="H186" s="31"/>
       <c r="I186" s="33" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="J186" s="33" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K186" s="31"/>
       <c r="L186" s="31" t="s">
@@ -13901,17 +13902,17 @@
       <c r="G187" s="31"/>
       <c r="H187" s="31"/>
       <c r="I187" s="33" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J187" s="33" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="K187" s="31"/>
       <c r="L187" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M187" s="33" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="N187" s="31" t="s">
         <v>85</v>
@@ -13926,7 +13927,7 @@
         <v>274</v>
       </c>
       <c r="R187" s="33" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="S187" s="31"/>
       <c r="T187" s="31"/>
@@ -13949,17 +13950,17 @@
       <c r="G188" s="31"/>
       <c r="H188" s="31"/>
       <c r="I188" s="33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="J188" s="33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="K188" s="31"/>
       <c r="L188" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M188" s="33" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="N188" s="31" t="s">
         <v>85</v>
@@ -13974,7 +13975,7 @@
         <v>274</v>
       </c>
       <c r="R188" s="33" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="S188" s="31"/>
       <c r="T188" s="31"/>
@@ -13997,10 +13998,10 @@
       <c r="G189" s="31"/>
       <c r="H189" s="31"/>
       <c r="I189" s="33" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="J189" s="33" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="K189" s="31"/>
       <c r="L189" s="31" t="s">
@@ -14043,17 +14044,17 @@
       <c r="G190" s="31"/>
       <c r="H190" s="31"/>
       <c r="I190" s="33" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="J190" s="33" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K190" s="31"/>
       <c r="L190" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M190" s="33" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="N190" s="31" t="s">
         <v>85</v>
@@ -14068,7 +14069,7 @@
         <v>274</v>
       </c>
       <c r="R190" s="33" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="S190" s="31"/>
       <c r="T190" s="31"/>
@@ -14091,17 +14092,17 @@
       <c r="G191" s="31"/>
       <c r="H191" s="31"/>
       <c r="I191" s="33" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="J191" s="33" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K191" s="31"/>
       <c r="L191" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M191" s="33" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="N191" s="31" t="s">
         <v>85</v>
@@ -14116,7 +14117,7 @@
         <v>274</v>
       </c>
       <c r="R191" s="33" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="S191" s="31"/>
       <c r="T191" s="31"/>
@@ -14139,17 +14140,17 @@
       <c r="G192" s="31"/>
       <c r="H192" s="31"/>
       <c r="I192" s="33" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="J192" s="33" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K192" s="31"/>
       <c r="L192" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M192" s="33" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N192" s="31" t="s">
         <v>85</v>
@@ -14164,7 +14165,7 @@
         <v>274</v>
       </c>
       <c r="R192" s="33" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="S192" s="31"/>
       <c r="T192" s="31"/>
@@ -14187,17 +14188,17 @@
       <c r="G193" s="31"/>
       <c r="H193" s="31"/>
       <c r="I193" s="33" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="J193" s="33" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="K193" s="31"/>
       <c r="L193" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M193" s="33" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="N193" s="31" t="s">
         <v>85</v>
@@ -14212,7 +14213,7 @@
         <v>274</v>
       </c>
       <c r="R193" s="33" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="S193" s="31"/>
       <c r="T193" s="31"/>
@@ -14235,17 +14236,17 @@
       <c r="G194" s="31"/>
       <c r="H194" s="31"/>
       <c r="I194" s="31" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="J194" s="31" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="K194" s="31"/>
       <c r="L194" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M194" s="33" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="N194" s="31" t="s">
         <v>85</v>
@@ -14260,7 +14261,7 @@
         <v>274</v>
       </c>
       <c r="R194" s="33" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="S194" s="31"/>
       <c r="T194" s="31"/>
@@ -14283,17 +14284,17 @@
       <c r="G195" s="31"/>
       <c r="H195" s="31"/>
       <c r="I195" s="33" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J195" s="33" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="K195" s="31"/>
       <c r="L195" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M195" s="33" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="N195" s="31" t="s">
         <v>85</v>
@@ -14308,7 +14309,7 @@
         <v>274</v>
       </c>
       <c r="R195" s="33" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="S195" s="31"/>
       <c r="T195" s="31"/>
@@ -14331,17 +14332,17 @@
       <c r="G196" s="31"/>
       <c r="H196" s="31"/>
       <c r="I196" s="33" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J196" s="33" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="K196" s="31"/>
       <c r="L196" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M196" s="33" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="N196" s="31" t="s">
         <v>85</v>
@@ -14356,7 +14357,7 @@
         <v>274</v>
       </c>
       <c r="R196" s="33" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="S196" s="31"/>
       <c r="T196" s="31"/>
@@ -14379,17 +14380,17 @@
       <c r="G197" s="31"/>
       <c r="H197" s="31"/>
       <c r="I197" s="33" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J197" s="33" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="K197" s="31"/>
       <c r="L197" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M197" s="33" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="N197" s="31" t="s">
         <v>85</v>
@@ -14404,7 +14405,7 @@
         <v>274</v>
       </c>
       <c r="R197" s="33" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="S197" s="31"/>
       <c r="T197" s="31"/>
@@ -14427,17 +14428,17 @@
       <c r="G198" s="31"/>
       <c r="H198" s="31"/>
       <c r="I198" s="33" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="J198" s="33" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="K198" s="31"/>
       <c r="L198" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M198" s="33" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N198" s="31" t="s">
         <v>85</v>
@@ -14452,7 +14453,7 @@
         <v>274</v>
       </c>
       <c r="R198" s="33" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="S198" s="31"/>
       <c r="T198" s="31"/>
@@ -14475,17 +14476,17 @@
       <c r="G199" s="31"/>
       <c r="H199" s="31"/>
       <c r="I199" s="33" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="J199" s="33" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="K199" s="31"/>
       <c r="L199" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M199" s="33" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="N199" s="31" t="s">
         <v>85</v>
@@ -14500,7 +14501,7 @@
         <v>274</v>
       </c>
       <c r="R199" s="33" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="S199" s="31"/>
       <c r="T199" s="31"/>
@@ -14523,17 +14524,17 @@
       <c r="G200" s="31"/>
       <c r="H200" s="31"/>
       <c r="I200" s="33" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="J200" s="33" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="K200" s="31"/>
       <c r="L200" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M200" s="33" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="N200" s="31" t="s">
         <v>86</v>
@@ -14548,10 +14549,10 @@
         <v>274</v>
       </c>
       <c r="R200" s="33" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="S200" s="33" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="T200" s="31"/>
       <c r="U200" s="31"/>
@@ -14573,17 +14574,17 @@
       <c r="G201" s="31"/>
       <c r="H201" s="31"/>
       <c r="I201" s="33" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="J201" s="33" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="K201" s="31"/>
       <c r="L201" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M201" s="33" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="N201" s="31" t="s">
         <v>85</v>
@@ -14598,7 +14599,7 @@
         <v>274</v>
       </c>
       <c r="R201" s="33" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="S201" s="31"/>
       <c r="T201" s="31"/>
@@ -14621,17 +14622,17 @@
       <c r="G202" s="31"/>
       <c r="H202" s="31"/>
       <c r="I202" s="33" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J202" s="33" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K202" s="31"/>
       <c r="L202" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M202" s="33" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="N202" s="31" t="s">
         <v>85</v>
@@ -14646,7 +14647,7 @@
         <v>274</v>
       </c>
       <c r="R202" s="33" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="S202" s="31"/>
       <c r="T202" s="31"/>
@@ -14669,17 +14670,17 @@
       <c r="G203" s="31"/>
       <c r="H203" s="31"/>
       <c r="I203" s="33" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J203" s="33" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="K203" s="31"/>
       <c r="L203" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M203" s="33" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="N203" s="31" t="s">
         <v>85</v>
@@ -14694,7 +14695,7 @@
         <v>274</v>
       </c>
       <c r="R203" s="33" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="S203" s="31"/>
       <c r="T203" s="31"/>
@@ -14717,17 +14718,17 @@
       <c r="G204" s="31"/>
       <c r="H204" s="31"/>
       <c r="I204" s="33" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="J204" s="33" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="K204" s="31"/>
       <c r="L204" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M204" s="33" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="N204" s="31" t="s">
         <v>85</v>
@@ -14742,7 +14743,7 @@
         <v>274</v>
       </c>
       <c r="R204" s="33" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="S204" s="31"/>
       <c r="T204" s="31"/>
@@ -14765,17 +14766,17 @@
       <c r="G205" s="31"/>
       <c r="H205" s="31"/>
       <c r="I205" s="33" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J205" s="33" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K205" s="31"/>
       <c r="L205" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M205" s="33" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="N205" s="31" t="s">
         <v>85</v>
@@ -14790,7 +14791,7 @@
         <v>274</v>
       </c>
       <c r="R205" s="33" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="S205" s="31"/>
       <c r="T205" s="31"/>
@@ -14813,17 +14814,17 @@
       <c r="G206" s="31"/>
       <c r="H206" s="31"/>
       <c r="I206" s="33" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="J206" s="33" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="K206" s="31"/>
       <c r="L206" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M206" s="33" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="N206" s="31" t="s">
         <v>85</v>
@@ -14838,7 +14839,7 @@
         <v>274</v>
       </c>
       <c r="R206" s="33" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="S206" s="31"/>
       <c r="T206" s="31"/>
@@ -14861,17 +14862,17 @@
       <c r="G207" s="31"/>
       <c r="H207" s="31"/>
       <c r="I207" s="33" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="J207" s="33" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="K207" s="31"/>
       <c r="L207" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M207" s="33" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="N207" s="31" t="s">
         <v>85</v>
@@ -14886,7 +14887,7 @@
         <v>274</v>
       </c>
       <c r="R207" s="33" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="S207" s="31"/>
       <c r="T207" s="31"/>
@@ -14909,17 +14910,17 @@
       <c r="G208" s="31"/>
       <c r="H208" s="31"/>
       <c r="I208" s="33" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="J208" s="33" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="K208" s="31"/>
       <c r="L208" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M208" s="33" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="N208" s="31" t="s">
         <v>85</v>
@@ -14934,7 +14935,7 @@
         <v>274</v>
       </c>
       <c r="R208" s="33" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="S208" s="31"/>
       <c r="T208" s="31"/>
@@ -14957,17 +14958,17 @@
       <c r="G209" s="31"/>
       <c r="H209" s="31"/>
       <c r="I209" s="33" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="J209" s="33" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="K209" s="31"/>
       <c r="L209" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M209" s="33" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="N209" s="31" t="s">
         <v>85</v>
@@ -14982,7 +14983,7 @@
         <v>274</v>
       </c>
       <c r="R209" s="33" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="S209" s="31"/>
       <c r="T209" s="31"/>
@@ -15005,17 +15006,17 @@
       <c r="G210" s="31"/>
       <c r="H210" s="31"/>
       <c r="I210" s="33" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J210" s="33" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="K210" s="31"/>
       <c r="L210" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M210" s="33" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="N210" s="31" t="s">
         <v>84</v>
@@ -15027,7 +15028,7 @@
         <v>94</v>
       </c>
       <c r="Q210" s="33" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="R210" s="31"/>
       <c r="S210" s="31"/>
@@ -15051,17 +15052,17 @@
       <c r="G211" s="31"/>
       <c r="H211" s="31"/>
       <c r="I211" s="33" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="J211" s="33" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="K211" s="31"/>
       <c r="L211" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M211" s="33" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="N211" s="31" t="s">
         <v>85</v>
@@ -15076,7 +15077,7 @@
         <v>199</v>
       </c>
       <c r="R211" s="33" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="S211" s="31"/>
       <c r="T211" s="31"/>
@@ -15099,10 +15100,10 @@
       <c r="G212" s="31"/>
       <c r="H212" s="31"/>
       <c r="I212" s="33" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J212" s="33" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="K212" s="31"/>
       <c r="L212" s="31" t="s">
@@ -15145,10 +15146,10 @@
       <c r="G213" s="31"/>
       <c r="H213" s="31"/>
       <c r="I213" s="33" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J213" s="33" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="K213" s="31"/>
       <c r="L213" s="31" t="s">
@@ -15191,10 +15192,10 @@
       <c r="G214" s="31"/>
       <c r="H214" s="31"/>
       <c r="I214" s="33" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="J214" s="33" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="K214" s="31"/>
       <c r="L214" s="31" t="s">
@@ -15237,17 +15238,17 @@
       <c r="G215" s="31"/>
       <c r="H215" s="31"/>
       <c r="I215" s="33" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="J215" s="33" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="K215" s="31"/>
       <c r="L215" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M215" s="33" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="N215" s="31" t="s">
         <v>85</v>
@@ -15262,7 +15263,7 @@
         <v>199</v>
       </c>
       <c r="R215" s="33" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="S215" s="31"/>
       <c r="T215" s="31"/>
@@ -15285,17 +15286,17 @@
       <c r="G216" s="31"/>
       <c r="H216" s="31"/>
       <c r="I216" s="33" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="J216" s="33" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="K216" s="31"/>
       <c r="L216" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M216" s="33" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="N216" s="31" t="s">
         <v>85</v>
@@ -15310,7 +15311,7 @@
         <v>199</v>
       </c>
       <c r="R216" s="33" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="S216" s="31"/>
       <c r="T216" s="31"/>
@@ -15333,10 +15334,10 @@
       <c r="G217" s="31"/>
       <c r="H217" s="31"/>
       <c r="I217" s="33" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="J217" s="33" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="K217" s="31"/>
       <c r="L217" s="31" t="s">
@@ -15379,17 +15380,17 @@
       <c r="G218" s="31"/>
       <c r="H218" s="31"/>
       <c r="I218" s="33" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="J218" s="33" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="K218" s="31"/>
       <c r="L218" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M218" s="33" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="N218" s="31" t="s">
         <v>85</v>
@@ -15404,7 +15405,7 @@
         <v>199</v>
       </c>
       <c r="R218" s="33" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="S218" s="31"/>
       <c r="T218" s="31"/>
@@ -15427,17 +15428,17 @@
       <c r="G219" s="31"/>
       <c r="H219" s="31"/>
       <c r="I219" s="33" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="J219" s="33" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="K219" s="31"/>
       <c r="L219" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M219" s="33" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="N219" s="31" t="s">
         <v>85</v>
@@ -15452,7 +15453,7 @@
         <v>199</v>
       </c>
       <c r="R219" s="33" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="S219" s="31"/>
       <c r="T219" s="31"/>
@@ -15475,17 +15476,17 @@
       <c r="G220" s="31"/>
       <c r="H220" s="31"/>
       <c r="I220" s="33" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="J220" s="33" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="K220" s="31"/>
       <c r="L220" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M220" s="33" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="N220" s="31" t="s">
         <v>85</v>
@@ -15500,7 +15501,7 @@
         <v>199</v>
       </c>
       <c r="R220" s="33" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="S220" s="31"/>
       <c r="T220" s="31"/>
@@ -15523,17 +15524,17 @@
       <c r="G221" s="31"/>
       <c r="H221" s="31"/>
       <c r="I221" s="33" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="J221" s="33" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="K221" s="31"/>
       <c r="L221" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M221" s="33" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="N221" s="31" t="s">
         <v>85</v>
@@ -15548,7 +15549,7 @@
         <v>199</v>
       </c>
       <c r="R221" s="33" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="S221" s="31"/>
       <c r="T221" s="31"/>
@@ -15571,17 +15572,17 @@
       <c r="G222" s="31"/>
       <c r="H222" s="31"/>
       <c r="I222" s="33" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="J222" s="33" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="K222" s="31"/>
       <c r="L222" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M222" s="33" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="N222" s="31" t="s">
         <v>85</v>
@@ -15596,7 +15597,7 @@
         <v>199</v>
       </c>
       <c r="R222" s="33" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="S222" s="31"/>
       <c r="T222" s="31"/>
@@ -15619,17 +15620,17 @@
       <c r="G223" s="31"/>
       <c r="H223" s="31"/>
       <c r="I223" s="33" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="J223" s="33" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K223" s="31"/>
       <c r="L223" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M223" s="33" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="N223" s="31" t="s">
         <v>85</v>
@@ -15644,7 +15645,7 @@
         <v>199</v>
       </c>
       <c r="R223" s="33" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="S223" s="31"/>
       <c r="T223" s="31"/>
@@ -15667,17 +15668,17 @@
       <c r="G224" s="31"/>
       <c r="H224" s="31"/>
       <c r="I224" s="33" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J224" s="33" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="K224" s="31"/>
       <c r="L224" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M224" s="33" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="N224" s="31" t="s">
         <v>85</v>
@@ -15692,7 +15693,7 @@
         <v>199</v>
       </c>
       <c r="R224" s="33" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="S224" s="31"/>
       <c r="T224" s="31"/>
@@ -15715,17 +15716,17 @@
       <c r="G225" s="31"/>
       <c r="H225" s="31"/>
       <c r="I225" s="33" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="J225" s="33" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="K225" s="31"/>
       <c r="L225" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M225" s="33" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="N225" s="31" t="s">
         <v>85</v>
@@ -15740,7 +15741,7 @@
         <v>279</v>
       </c>
       <c r="R225" s="33" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="S225" s="31"/>
       <c r="T225" s="31"/>
@@ -15763,17 +15764,17 @@
       <c r="G226" s="31"/>
       <c r="H226" s="31"/>
       <c r="I226" s="33" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="J226" s="33" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="K226" s="31"/>
       <c r="L226" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M226" s="33" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="N226" s="31" t="s">
         <v>85</v>
@@ -15788,7 +15789,7 @@
         <v>279</v>
       </c>
       <c r="R226" s="33" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="S226" s="31"/>
       <c r="T226" s="31"/>
@@ -15811,10 +15812,10 @@
       <c r="G227" s="31"/>
       <c r="H227" s="31"/>
       <c r="I227" s="33" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="J227" s="33" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="K227" s="31"/>
       <c r="L227" s="31" t="s">
@@ -15857,17 +15858,17 @@
       <c r="G228" s="31"/>
       <c r="H228" s="31"/>
       <c r="I228" s="33" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="J228" s="33" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="K228" s="31"/>
       <c r="L228" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M228" s="33" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="N228" s="31" t="s">
         <v>85</v>
@@ -15882,7 +15883,7 @@
         <v>279</v>
       </c>
       <c r="R228" s="33" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="S228" s="31"/>
       <c r="T228" s="31"/>
@@ -15905,17 +15906,17 @@
       <c r="G229" s="31"/>
       <c r="H229" s="31"/>
       <c r="I229" s="33" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="J229" s="33" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="K229" s="31"/>
       <c r="L229" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M229" s="31" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="N229" s="31" t="s">
         <v>87</v>
@@ -15930,13 +15931,13 @@
         <v>279</v>
       </c>
       <c r="R229" s="33" t="s">
+        <v>579</v>
+      </c>
+      <c r="S229" s="33" t="s">
         <v>580</v>
       </c>
-      <c r="S229" s="33" t="s">
+      <c r="T229" s="33" t="s">
         <v>581</v>
-      </c>
-      <c r="T229" s="33" t="s">
-        <v>582</v>
       </c>
       <c r="U229" s="31"/>
       <c r="V229" s="31"/>
@@ -15957,10 +15958,10 @@
       <c r="G230" s="31"/>
       <c r="H230" s="31"/>
       <c r="I230" s="33" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J230" s="33" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="K230" s="31"/>
       <c r="L230" s="31" t="s">
@@ -16003,17 +16004,17 @@
       <c r="G231" s="31"/>
       <c r="H231" s="31"/>
       <c r="I231" s="33" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J231" s="33" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="K231" s="31"/>
       <c r="L231" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M231" s="33" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="N231" s="31" t="s">
         <v>85</v>
@@ -16028,7 +16029,7 @@
         <v>226</v>
       </c>
       <c r="R231" s="33" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="S231" s="31"/>
       <c r="T231" s="31"/>
@@ -16051,17 +16052,17 @@
       <c r="G232" s="31"/>
       <c r="H232" s="31"/>
       <c r="I232" s="33" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J232" s="33" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="K232" s="31"/>
       <c r="L232" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M232" s="33" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="N232" s="31" t="s">
         <v>85</v>
@@ -16076,7 +16077,7 @@
         <v>226</v>
       </c>
       <c r="R232" s="33" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="S232" s="31"/>
       <c r="T232" s="31"/>
@@ -16099,17 +16100,17 @@
       <c r="G233" s="31"/>
       <c r="H233" s="31"/>
       <c r="I233" s="33" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="J233" s="33" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="K233" s="31"/>
       <c r="L233" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M233" s="33" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="N233" s="31" t="s">
         <v>85</v>
@@ -16124,7 +16125,7 @@
         <v>226</v>
       </c>
       <c r="R233" s="33" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="S233" s="31"/>
       <c r="T233" s="31"/>
@@ -16147,17 +16148,17 @@
       <c r="G234" s="31"/>
       <c r="H234" s="31"/>
       <c r="I234" s="33" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="J234" s="33" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="K234" s="31"/>
       <c r="L234" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M234" s="33" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="N234" s="31" t="s">
         <v>85</v>
@@ -16172,7 +16173,7 @@
         <v>226</v>
       </c>
       <c r="R234" s="33" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="S234" s="31"/>
       <c r="T234" s="31"/>
@@ -16195,17 +16196,17 @@
       <c r="G235" s="31"/>
       <c r="H235" s="31"/>
       <c r="I235" s="33" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="J235" s="33" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K235" s="31"/>
       <c r="L235" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M235" s="33" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="N235" s="31" t="s">
         <v>85</v>
@@ -16220,7 +16221,7 @@
         <v>226</v>
       </c>
       <c r="R235" s="33" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="S235" s="31"/>
       <c r="T235" s="31"/>
@@ -16243,10 +16244,10 @@
       <c r="G236" s="31"/>
       <c r="H236" s="31"/>
       <c r="I236" s="33" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="J236" s="33" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="K236" s="31"/>
       <c r="L236" s="31" t="s">
@@ -16289,17 +16290,17 @@
       <c r="G237" s="31"/>
       <c r="H237" s="31"/>
       <c r="I237" s="33" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="J237" s="33" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="K237" s="31"/>
       <c r="L237" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M237" s="33" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="N237" s="31" t="s">
         <v>85</v>
@@ -16314,7 +16315,7 @@
         <v>226</v>
       </c>
       <c r="R237" s="33" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="S237" s="31"/>
       <c r="T237" s="31"/>
@@ -16337,17 +16338,17 @@
       <c r="G238" s="31"/>
       <c r="H238" s="31"/>
       <c r="I238" s="33" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="J238" s="33" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="K238" s="31"/>
       <c r="L238" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M238" s="33" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="N238" s="31" t="s">
         <v>85</v>
@@ -16362,7 +16363,7 @@
         <v>226</v>
       </c>
       <c r="R238" s="33" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="S238" s="31"/>
       <c r="T238" s="31"/>
@@ -16385,10 +16386,10 @@
       <c r="G239" s="31"/>
       <c r="H239" s="31"/>
       <c r="I239" s="33" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J239" s="33" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="K239" s="31"/>
       <c r="L239" s="31" t="s">
@@ -16431,17 +16432,17 @@
       <c r="G240" s="31"/>
       <c r="H240" s="31"/>
       <c r="I240" s="33" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J240" s="33" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="K240" s="31"/>
       <c r="L240" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M240" s="33" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="N240" s="31" t="s">
         <v>85</v>
@@ -16456,7 +16457,7 @@
         <v>226</v>
       </c>
       <c r="R240" s="33" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="S240" s="31"/>
       <c r="T240" s="31"/>
@@ -16479,17 +16480,17 @@
       <c r="G241" s="31"/>
       <c r="H241" s="31"/>
       <c r="I241" s="33" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="J241" s="33" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="K241" s="31"/>
       <c r="L241" s="31" t="s">
         <v>208</v>
       </c>
       <c r="M241" s="33" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="N241" s="31" t="s">
         <v>85</v>
@@ -16504,7 +16505,7 @@
         <v>226</v>
       </c>
       <c r="R241" s="33" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="S241" s="31"/>
       <c r="T241" s="31"/>
@@ -16527,10 +16528,10 @@
       <c r="G242" s="31"/>
       <c r="H242" s="31"/>
       <c r="I242" s="33" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="J242" s="33" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="K242" s="31"/>
       <c r="L242" s="31" t="s">
@@ -16575,10 +16576,10 @@
       <c r="G243" s="31"/>
       <c r="H243" s="31"/>
       <c r="I243" s="33" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="J243" s="33" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="K243" s="31"/>
       <c r="L243" s="31" t="s">
@@ -16621,17 +16622,17 @@
       <c r="G244" s="31"/>
       <c r="H244" s="31"/>
       <c r="I244" s="33" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="J244" s="33" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="K244" s="31"/>
       <c r="L244" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M244" s="33" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="N244" s="31" t="s">
         <v>84</v>
@@ -16643,7 +16644,7 @@
         <v>94</v>
       </c>
       <c r="Q244" s="33" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="R244" s="31"/>
       <c r="S244" s="31"/>
@@ -16667,17 +16668,17 @@
       <c r="G245" s="31"/>
       <c r="H245" s="31"/>
       <c r="I245" s="33" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="J245" s="33" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="K245" s="31"/>
       <c r="L245" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M245" s="33" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="N245" s="31" t="s">
         <v>84</v>
@@ -16689,7 +16690,7 @@
         <v>94</v>
       </c>
       <c r="Q245" s="33" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="R245" s="31"/>
       <c r="S245" s="31"/>
@@ -16713,17 +16714,17 @@
       <c r="G246" s="31"/>
       <c r="H246" s="31"/>
       <c r="I246" s="33" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="J246" s="33" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="K246" s="31"/>
       <c r="L246" s="31" t="s">
         <v>294</v>
       </c>
       <c r="M246" s="33" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="N246" s="31" t="s">
         <v>84</v>
@@ -16735,7 +16736,7 @@
         <v>94</v>
       </c>
       <c r="Q246" s="33" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="R246" s="31"/>
       <c r="S246" s="31"/>
@@ -16759,17 +16760,17 @@
       <c r="G247" s="31"/>
       <c r="H247" s="31"/>
       <c r="I247" s="33" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="J247" s="33" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="K247" s="31"/>
       <c r="L247" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M247" s="33" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="N247" s="31" t="s">
         <v>85</v>
@@ -16781,10 +16782,10 @@
         <v>94</v>
       </c>
       <c r="Q247" s="33" t="s">
+        <v>603</v>
+      </c>
+      <c r="R247" s="33" t="s">
         <v>604</v>
-      </c>
-      <c r="R247" s="33" t="s">
-        <v>605</v>
       </c>
       <c r="S247" s="31"/>
       <c r="T247" s="31"/>
@@ -16807,17 +16808,17 @@
       <c r="G248" s="31"/>
       <c r="H248" s="31"/>
       <c r="I248" s="33" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J248" s="33" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="K248" s="31"/>
       <c r="L248" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M248" s="33" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="N248" s="31" t="s">
         <v>85</v>
@@ -16832,7 +16833,7 @@
         <v>268</v>
       </c>
       <c r="R248" s="33" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="S248" s="31"/>
       <c r="T248" s="31"/>
@@ -16855,10 +16856,10 @@
       <c r="G249" s="31"/>
       <c r="H249" s="31"/>
       <c r="I249" s="33" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="J249" s="33" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="K249" s="31"/>
       <c r="L249" s="31" t="s">
@@ -16901,17 +16902,17 @@
       <c r="G250" s="31"/>
       <c r="H250" s="31"/>
       <c r="I250" s="33" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="J250" s="33" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="K250" s="31"/>
       <c r="L250" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M250" s="33" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="N250" s="31" t="s">
         <v>85</v>
@@ -16926,7 +16927,7 @@
         <v>268</v>
       </c>
       <c r="R250" s="33" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="S250" s="31"/>
       <c r="T250" s="31"/>
@@ -16949,10 +16950,10 @@
       <c r="G251" s="31"/>
       <c r="H251" s="31"/>
       <c r="I251" s="33" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="J251" s="33" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="K251" s="31"/>
       <c r="L251" s="31" t="s">
@@ -16995,17 +16996,17 @@
       <c r="G252" s="31"/>
       <c r="H252" s="31"/>
       <c r="I252" s="33" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="J252" s="33" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="K252" s="31"/>
       <c r="L252" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M252" s="33" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="N252" s="31" t="s">
         <v>85</v>
@@ -17020,7 +17021,7 @@
         <v>268</v>
       </c>
       <c r="R252" s="33" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="S252" s="31"/>
       <c r="T252" s="31"/>
@@ -17043,17 +17044,17 @@
       <c r="G253" s="31"/>
       <c r="H253" s="31"/>
       <c r="I253" s="33" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="J253" s="33" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="K253" s="31"/>
       <c r="L253" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M253" s="33" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="N253" s="31" t="s">
         <v>84</v>
@@ -17065,7 +17066,7 @@
         <v>94</v>
       </c>
       <c r="Q253" s="33" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="R253" s="31"/>
       <c r="S253" s="31"/>
@@ -17089,17 +17090,17 @@
       <c r="G254" s="31"/>
       <c r="H254" s="31"/>
       <c r="I254" s="33" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="J254" s="33" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="K254" s="31"/>
       <c r="L254" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M254" s="33" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="N254" s="31" t="s">
         <v>84</v>
@@ -17111,7 +17112,7 @@
         <v>94</v>
       </c>
       <c r="Q254" s="33" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="R254" s="31"/>
       <c r="S254" s="31"/>
@@ -17135,17 +17136,17 @@
       <c r="G255" s="31"/>
       <c r="H255" s="31"/>
       <c r="I255" s="33" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J255" s="33" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K255" s="31"/>
       <c r="L255" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M255" s="33" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="N255" s="31" t="s">
         <v>84</v>
@@ -17157,7 +17158,7 @@
         <v>94</v>
       </c>
       <c r="Q255" s="33" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="R255" s="31"/>
       <c r="S255" s="31"/>
@@ -17181,10 +17182,10 @@
       <c r="G256" s="31"/>
       <c r="H256" s="31"/>
       <c r="I256" s="33" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="J256" s="33" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="K256" s="31"/>
       <c r="L256" s="31" t="s">
@@ -17227,10 +17228,10 @@
       <c r="G257" s="31"/>
       <c r="H257" s="31"/>
       <c r="I257" s="33" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="J257" s="33" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="K257" s="31"/>
       <c r="L257" s="31" t="s">
@@ -17275,17 +17276,17 @@
       <c r="G258" s="31"/>
       <c r="H258" s="31"/>
       <c r="I258" s="33" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="J258" s="33" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="K258" s="31"/>
       <c r="L258" s="31" t="s">
         <v>209</v>
       </c>
       <c r="M258" s="33" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="N258" s="31" t="s">
         <v>85</v>
@@ -17300,7 +17301,7 @@
         <v>247</v>
       </c>
       <c r="R258" s="33" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="S258" s="31"/>
       <c r="T258" s="31"/>
@@ -17323,10 +17324,10 @@
       <c r="G259" s="31"/>
       <c r="H259" s="31"/>
       <c r="I259" s="33" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="J259" s="33" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="K259" s="31"/>
       <c r="L259" s="31" t="s">
@@ -17369,10 +17370,10 @@
       <c r="G260" s="31"/>
       <c r="H260" s="31"/>
       <c r="I260" s="33" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="J260" s="33" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="K260" s="31"/>
       <c r="L260" s="31" t="s">
@@ -17417,10 +17418,10 @@
       <c r="G261" s="31"/>
       <c r="H261" s="31"/>
       <c r="I261" s="33" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="J261" s="33" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="K261" s="31"/>
       <c r="L261" s="31" t="s">
@@ -17461,10 +17462,10 @@
       <c r="G262" s="31"/>
       <c r="H262" s="31"/>
       <c r="I262" s="33" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="J262" s="33" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="K262" s="31"/>
       <c r="L262" s="31" t="s">
@@ -17507,17 +17508,17 @@
       <c r="G263" s="31"/>
       <c r="H263" s="31"/>
       <c r="I263" s="33" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="J263" s="33" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="K263" s="31"/>
       <c r="L263" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M263" s="33" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="N263" s="31" t="s">
         <v>86</v>
@@ -17532,10 +17533,10 @@
         <v>223</v>
       </c>
       <c r="R263" s="33" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="S263" s="33" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="T263" s="31"/>
       <c r="U263" s="31">
@@ -17559,17 +17560,17 @@
       <c r="G264" s="31"/>
       <c r="H264" s="31"/>
       <c r="I264" s="33" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="J264" s="33" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="K264" s="31"/>
       <c r="L264" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M264" s="33" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="N264" s="31" t="s">
         <v>86</v>
@@ -17584,10 +17585,10 @@
         <v>223</v>
       </c>
       <c r="R264" s="33" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="S264" s="33" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="T264" s="31"/>
       <c r="U264" s="31">
@@ -17611,17 +17612,17 @@
       <c r="G265" s="31"/>
       <c r="H265" s="31"/>
       <c r="I265" s="33" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="J265" s="33" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="K265" s="31"/>
       <c r="L265" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M265" s="33" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="N265" s="31" t="s">
         <v>86</v>
@@ -17636,10 +17637,10 @@
         <v>223</v>
       </c>
       <c r="R265" s="33" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="S265" s="33" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="T265" s="31"/>
       <c r="U265" s="31"/>
@@ -17661,17 +17662,17 @@
       <c r="G266" s="31"/>
       <c r="H266" s="31"/>
       <c r="I266" s="33" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J266" s="33" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="K266" s="31"/>
       <c r="L266" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M266" s="33" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="N266" s="31" t="s">
         <v>85</v>
@@ -17680,13 +17681,13 @@
         <v>93</v>
       </c>
       <c r="P266" s="33" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="Q266" s="33" t="s">
         <v>223</v>
       </c>
       <c r="R266" s="33" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="S266" s="31"/>
       <c r="T266" s="31"/>
@@ -17711,10 +17712,10 @@
       <c r="G267" s="31"/>
       <c r="H267" s="31"/>
       <c r="I267" s="33" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="J267" s="33" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="K267" s="31"/>
       <c r="L267" s="31" t="s">
@@ -17757,17 +17758,17 @@
       <c r="G268" s="31"/>
       <c r="H268" s="31"/>
       <c r="I268" s="33" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="J268" s="33" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="K268" s="31"/>
       <c r="L268" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M268" s="33" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="N268" s="31" t="s">
         <v>87</v>
@@ -17782,13 +17783,13 @@
         <v>144</v>
       </c>
       <c r="R268" s="33" t="s">
+        <v>633</v>
+      </c>
+      <c r="S268" s="33" t="s">
+        <v>632</v>
+      </c>
+      <c r="T268" s="33" t="s">
         <v>634</v>
-      </c>
-      <c r="S268" s="33" t="s">
-        <v>633</v>
-      </c>
-      <c r="T268" s="33" t="s">
-        <v>635</v>
       </c>
       <c r="U268" s="31"/>
       <c r="V268" s="31"/>
@@ -17809,10 +17810,10 @@
       <c r="G269" s="31"/>
       <c r="H269" s="31"/>
       <c r="I269" s="33" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="J269" s="33" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="K269" s="31"/>
       <c r="L269" s="31" t="s">
@@ -17855,17 +17856,17 @@
       <c r="G270" s="31"/>
       <c r="H270" s="31"/>
       <c r="I270" s="33" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="J270" s="33" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="K270" s="31"/>
       <c r="L270" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M270" s="33" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="N270" s="31" t="s">
         <v>86</v>
@@ -17880,10 +17881,10 @@
         <v>144</v>
       </c>
       <c r="R270" s="33" t="s">
+        <v>638</v>
+      </c>
+      <c r="S270" s="33" t="s">
         <v>639</v>
-      </c>
-      <c r="S270" s="33" t="s">
-        <v>640</v>
       </c>
       <c r="T270" s="31"/>
       <c r="U270" s="31"/>
@@ -17905,17 +17906,17 @@
       <c r="G271" s="31"/>
       <c r="H271" s="31"/>
       <c r="I271" s="33" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="J271" s="33" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="K271" s="31"/>
       <c r="L271" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M271" s="33" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="N271" s="31" t="s">
         <v>86</v>
@@ -17930,10 +17931,10 @@
         <v>144</v>
       </c>
       <c r="R271" s="33" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="S271" s="33" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="T271" s="31"/>
       <c r="U271" s="31"/>
@@ -17955,10 +17956,10 @@
       <c r="G272" s="31"/>
       <c r="H272" s="31"/>
       <c r="I272" s="33" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="J272" s="33" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="K272" s="31"/>
       <c r="L272" s="31" t="s">
@@ -18001,17 +18002,17 @@
       <c r="G273" s="31"/>
       <c r="H273" s="31"/>
       <c r="I273" s="33" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J273" s="33" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="K273" s="31"/>
       <c r="L273" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M273" s="33" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="N273" s="31" t="s">
         <v>86</v>
@@ -18026,10 +18027,10 @@
         <v>144</v>
       </c>
       <c r="R273" s="33" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="S273" s="33" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="T273" s="31"/>
       <c r="U273" s="31"/>
@@ -18051,17 +18052,17 @@
       <c r="G274" s="31"/>
       <c r="H274" s="31"/>
       <c r="I274" s="33" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J274" s="33" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="K274" s="31"/>
       <c r="L274" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M274" s="31" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="N274" s="31" t="s">
         <v>87</v>
@@ -18076,13 +18077,13 @@
         <v>144</v>
       </c>
       <c r="R274" s="33" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="S274" s="33" t="s">
+        <v>645</v>
+      </c>
+      <c r="T274" s="33" t="s">
         <v>646</v>
-      </c>
-      <c r="T274" s="33" t="s">
-        <v>647</v>
       </c>
       <c r="U274" s="31"/>
       <c r="V274" s="31"/>
@@ -18103,17 +18104,17 @@
       <c r="G275" s="31"/>
       <c r="H275" s="31"/>
       <c r="I275" s="33" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J275" s="33" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="K275" s="31"/>
       <c r="L275" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M275" s="33" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="N275" s="31" t="s">
         <v>86</v>
@@ -18128,10 +18129,10 @@
         <v>144</v>
       </c>
       <c r="R275" s="33" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="S275" s="33" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="T275" s="31"/>
       <c r="U275" s="31"/>
@@ -18153,17 +18154,17 @@
       <c r="G276" s="31"/>
       <c r="H276" s="31"/>
       <c r="I276" s="33" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J276" s="33" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="K276" s="31"/>
       <c r="L276" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M276" s="33" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="N276" s="31" t="s">
         <v>86</v>
@@ -18178,10 +18179,10 @@
         <v>144</v>
       </c>
       <c r="R276" s="33" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="S276" s="33" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="T276" s="31"/>
       <c r="U276" s="31"/>
@@ -18203,17 +18204,17 @@
       <c r="G277" s="31"/>
       <c r="H277" s="31"/>
       <c r="I277" s="33" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J277" s="33" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="K277" s="31"/>
       <c r="L277" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M277" s="33" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="N277" s="31" t="s">
         <v>85</v>
@@ -18228,7 +18229,7 @@
         <v>229</v>
       </c>
       <c r="R277" s="33" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="S277" s="31"/>
       <c r="T277" s="31"/>
@@ -18251,17 +18252,17 @@
       <c r="G278" s="31"/>
       <c r="H278" s="31"/>
       <c r="I278" s="33" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J278" s="33" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="K278" s="31"/>
       <c r="L278" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M278" s="31" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="N278" s="31" t="s">
         <v>87</v>
@@ -18276,13 +18277,13 @@
         <v>229</v>
       </c>
       <c r="R278" s="33" t="s">
+        <v>652</v>
+      </c>
+      <c r="S278" s="33" t="s">
+        <v>651</v>
+      </c>
+      <c r="T278" s="33" t="s">
         <v>653</v>
-      </c>
-      <c r="S278" s="33" t="s">
-        <v>652</v>
-      </c>
-      <c r="T278" s="33" t="s">
-        <v>654</v>
       </c>
       <c r="U278" s="31"/>
       <c r="V278" s="31"/>
@@ -18303,17 +18304,17 @@
       <c r="G279" s="31"/>
       <c r="H279" s="31"/>
       <c r="I279" s="33" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="J279" s="33" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="K279" s="31"/>
       <c r="L279" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M279" s="33" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="N279" s="31" t="s">
         <v>86</v>
@@ -18328,10 +18329,10 @@
         <v>229</v>
       </c>
       <c r="R279" s="33" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="S279" s="33" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="T279" s="31"/>
       <c r="U279" s="31"/>
@@ -18353,17 +18354,17 @@
       <c r="G280" s="31"/>
       <c r="H280" s="31"/>
       <c r="I280" s="33" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J280" s="33" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="K280" s="31"/>
       <c r="L280" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M280" s="33" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="N280" s="31" t="s">
         <v>85</v>
@@ -18378,7 +18379,7 @@
         <v>229</v>
       </c>
       <c r="R280" s="33" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="S280" s="31"/>
       <c r="T280" s="31"/>
@@ -18401,10 +18402,10 @@
       <c r="G281" s="31"/>
       <c r="H281" s="31"/>
       <c r="I281" s="33" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="J281" s="33" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="K281" s="31"/>
       <c r="L281" s="31" t="s">
@@ -18447,10 +18448,10 @@
       <c r="G282" s="31"/>
       <c r="H282" s="31"/>
       <c r="I282" s="33" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="J282" s="33" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="K282" s="31"/>
       <c r="L282" s="31" t="s">
@@ -18489,17 +18490,17 @@
       <c r="C283" s="31"/>
       <c r="H283" s="31"/>
       <c r="I283" s="33" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="J283" s="33" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="K283" s="31"/>
       <c r="L283" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M283" s="31" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="N283" s="31" t="s">
         <v>87</v>
@@ -18517,10 +18518,10 @@
         <v>220</v>
       </c>
       <c r="S283" s="33" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="T283" s="33" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="U283" s="31">
         <v>1993</v>
@@ -18537,29 +18538,29 @@
       <c r="A284" s="34"/>
       <c r="B284" s="34"/>
       <c r="C284" s="34" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D284" s="31"/>
       <c r="E284" s="31" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F284" s="31"/>
       <c r="G284" s="31" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="H284" s="31"/>
       <c r="I284" s="33" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="J284" s="33" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="K284" s="31"/>
       <c r="L284" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M284" s="31" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="N284" s="31" t="s">
         <v>87</v>
@@ -18580,7 +18581,7 @@
         <v>221</v>
       </c>
       <c r="T284" s="31" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="U284" s="31">
         <v>1997</v>
@@ -18599,29 +18600,29 @@
       <c r="A285" s="34"/>
       <c r="B285" s="34"/>
       <c r="C285" s="34" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D285" s="31"/>
       <c r="E285" s="31" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="F285" s="31"/>
       <c r="G285" s="31" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="H285" s="31"/>
       <c r="I285" s="33" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="J285" s="33" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="K285" s="31"/>
       <c r="L285" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M285" s="31" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="N285" s="31" t="s">
         <v>87</v>
@@ -18639,10 +18640,10 @@
         <v>220</v>
       </c>
       <c r="S285" s="31" t="s">
+        <v>668</v>
+      </c>
+      <c r="T285" s="31" t="s">
         <v>669</v>
-      </c>
-      <c r="T285" s="31" t="s">
-        <v>670</v>
       </c>
       <c r="U285" s="31"/>
       <c r="V285" s="31">
@@ -18659,29 +18660,29 @@
       <c r="A286" s="34"/>
       <c r="B286" s="34"/>
       <c r="C286" s="34" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="D286" s="31"/>
       <c r="E286" s="31" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="F286" s="31"/>
       <c r="G286" s="31" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="H286" s="31"/>
       <c r="I286" s="33" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="J286" s="33" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="K286" s="31"/>
       <c r="L286" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M286" s="31" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="N286" s="31" t="s">
         <v>87</v>
@@ -18699,10 +18700,10 @@
         <v>220</v>
       </c>
       <c r="S286" s="31" t="s">
+        <v>672</v>
+      </c>
+      <c r="T286" s="31" t="s">
         <v>673</v>
-      </c>
-      <c r="T286" s="31" t="s">
-        <v>674</v>
       </c>
       <c r="U286" s="31">
         <v>1977</v>
@@ -18721,22 +18722,22 @@
       <c r="A287" s="34"/>
       <c r="B287" s="34"/>
       <c r="C287" s="34" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D287" s="31"/>
       <c r="E287" s="31" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="F287" s="31"/>
       <c r="G287" s="31" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="H287" s="31"/>
       <c r="I287" s="33" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="J287" s="33" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="K287" s="31"/>
       <c r="L287" s="31" t="s">
@@ -18779,10 +18780,10 @@
       <c r="G288" s="31"/>
       <c r="H288" s="31"/>
       <c r="I288" s="33" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="J288" s="33" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="K288" s="31"/>
       <c r="L288" s="31" t="s">
@@ -18819,29 +18820,29 @@
       <c r="A289" s="34"/>
       <c r="B289" s="34"/>
       <c r="C289" s="34" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D289" s="31"/>
       <c r="E289" s="31" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F289" s="31"/>
       <c r="G289" s="31" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="H289" s="31"/>
       <c r="I289" s="33" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="J289" s="33" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="K289" s="31"/>
       <c r="L289" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M289" s="31" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="N289" s="31" t="s">
         <v>87</v>
@@ -18859,10 +18860,10 @@
         <v>220</v>
       </c>
       <c r="S289" s="33" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="T289" s="33" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="U289" s="31">
         <v>1993</v>
@@ -18887,10 +18888,10 @@
       <c r="G290" s="31"/>
       <c r="H290" s="31"/>
       <c r="I290" s="33" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="J290" s="33" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="K290" s="31"/>
       <c r="L290" s="31" t="s">
@@ -18931,38 +18932,38 @@
       <c r="G291" s="31"/>
       <c r="H291" s="31"/>
       <c r="I291" s="33" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="J291" s="33" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="K291" s="31"/>
       <c r="L291" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M291" s="33" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N291" s="31" t="s">
         <v>87</v>
       </c>
       <c r="O291" s="33" t="s">
+        <v>678</v>
+      </c>
+      <c r="P291" s="33" t="s">
         <v>679</v>
       </c>
-      <c r="P291" s="33" t="s">
+      <c r="Q291" s="33" t="s">
         <v>680</v>
       </c>
-      <c r="Q291" s="33" t="s">
+      <c r="R291" s="33" t="s">
         <v>681</v>
       </c>
-      <c r="R291" s="33" t="s">
+      <c r="S291" s="33" t="s">
         <v>682</v>
       </c>
-      <c r="S291" s="33" t="s">
-        <v>683</v>
-      </c>
       <c r="T291" s="33" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="U291" s="31"/>
       <c r="V291" s="31"/>
@@ -18983,10 +18984,10 @@
       <c r="G292" s="31"/>
       <c r="H292" s="31"/>
       <c r="I292" s="33" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="J292" s="33" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="K292" s="31"/>
       <c r="L292" s="31" t="s">
@@ -19025,17 +19026,17 @@
       <c r="G293" s="31"/>
       <c r="H293" s="31"/>
       <c r="I293" s="33" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="J293" s="33" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="K293" s="31"/>
       <c r="L293" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M293" s="33" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="N293" s="31" t="s">
         <v>86</v>
@@ -19047,13 +19048,13 @@
         <v>263</v>
       </c>
       <c r="Q293" s="33" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="R293" s="33" t="s">
+        <v>687</v>
+      </c>
+      <c r="S293" s="33" t="s">
         <v>688</v>
-      </c>
-      <c r="S293" s="33" t="s">
-        <v>689</v>
       </c>
       <c r="T293" s="31"/>
       <c r="U293" s="31"/>
@@ -19075,10 +19076,10 @@
       <c r="G294" s="31"/>
       <c r="H294" s="31"/>
       <c r="I294" s="33" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="J294" s="33" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="K294" s="31"/>
       <c r="L294" s="31" t="s">
@@ -19117,17 +19118,17 @@
       <c r="G295" s="31"/>
       <c r="H295" s="31"/>
       <c r="I295" s="33" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="J295" s="33" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="K295" s="31"/>
       <c r="L295" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M295" s="33" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="N295" s="31" t="s">
         <v>86</v>
@@ -19139,13 +19140,13 @@
         <v>263</v>
       </c>
       <c r="Q295" s="33" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="R295" s="33" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="S295" s="33" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="T295" s="31"/>
       <c r="U295" s="31"/>
@@ -19167,17 +19168,17 @@
       <c r="G296" s="31"/>
       <c r="H296" s="31"/>
       <c r="I296" s="33" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="J296" s="33" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="K296" s="31"/>
       <c r="L296" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M296" s="33" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="N296" s="31" t="s">
         <v>86</v>
@@ -19186,16 +19187,16 @@
         <v>262</v>
       </c>
       <c r="P296" s="33" t="s">
+        <v>697</v>
+      </c>
+      <c r="Q296" s="33" t="s">
         <v>698</v>
       </c>
-      <c r="Q296" s="33" t="s">
-        <v>699</v>
-      </c>
       <c r="R296" s="33" t="s">
+        <v>695</v>
+      </c>
+      <c r="S296" s="33" t="s">
         <v>696</v>
-      </c>
-      <c r="S296" s="33" t="s">
-        <v>697</v>
       </c>
       <c r="T296" s="31"/>
       <c r="U296" s="31"/>
@@ -19217,17 +19218,17 @@
       <c r="G297" s="31"/>
       <c r="H297" s="31"/>
       <c r="I297" s="33" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="J297" s="33" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="K297" s="31"/>
       <c r="L297" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M297" s="33" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="N297" s="31" t="s">
         <v>87</v>
@@ -19239,16 +19240,16 @@
         <v>302</v>
       </c>
       <c r="Q297" s="33" t="s">
+        <v>700</v>
+      </c>
+      <c r="R297" s="33" t="s">
         <v>701</v>
       </c>
-      <c r="R297" s="33" t="s">
+      <c r="S297" s="33" t="s">
+        <v>699</v>
+      </c>
+      <c r="T297" s="33" t="s">
         <v>702</v>
-      </c>
-      <c r="S297" s="33" t="s">
-        <v>700</v>
-      </c>
-      <c r="T297" s="33" t="s">
-        <v>703</v>
       </c>
       <c r="U297" s="31"/>
       <c r="V297" s="31"/>
@@ -19269,10 +19270,10 @@
       <c r="G298" s="31"/>
       <c r="H298" s="31"/>
       <c r="I298" s="33" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="J298" s="33" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="K298" s="31"/>
       <c r="L298" s="31" t="s">
@@ -19313,17 +19314,17 @@
       <c r="G299" s="31"/>
       <c r="H299" s="31"/>
       <c r="I299" s="33" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="J299" s="33" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="K299" s="31"/>
       <c r="L299" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M299" s="33" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="N299" s="31" t="s">
         <v>87</v>
@@ -19335,16 +19336,16 @@
         <v>302</v>
       </c>
       <c r="Q299" s="33" t="s">
+        <v>706</v>
+      </c>
+      <c r="R299" s="33" t="s">
         <v>707</v>
       </c>
-      <c r="R299" s="33" t="s">
+      <c r="S299" s="33" t="s">
+        <v>705</v>
+      </c>
+      <c r="T299" s="33" t="s">
         <v>708</v>
-      </c>
-      <c r="S299" s="33" t="s">
-        <v>706</v>
-      </c>
-      <c r="T299" s="33" t="s">
-        <v>709</v>
       </c>
       <c r="U299" s="31"/>
       <c r="V299" s="31"/>
@@ -19365,10 +19366,10 @@
       <c r="G300" s="31"/>
       <c r="H300" s="31"/>
       <c r="I300" s="33" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="J300" s="33" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="K300" s="31"/>
       <c r="L300" s="31" t="s">
@@ -19409,10 +19410,10 @@
       <c r="G301" s="31"/>
       <c r="H301" s="31"/>
       <c r="I301" s="33" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="J301" s="33" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="K301" s="31"/>
       <c r="L301" s="31" t="s">
@@ -19453,17 +19454,17 @@
       <c r="G302" s="31"/>
       <c r="H302" s="31"/>
       <c r="I302" s="33" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="J302" s="33" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="K302" s="31"/>
       <c r="L302" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M302" s="33" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="N302" s="31" t="s">
         <v>86</v>
@@ -19472,16 +19473,16 @@
         <v>241</v>
       </c>
       <c r="P302" s="33" t="s">
+        <v>712</v>
+      </c>
+      <c r="Q302" s="33" t="s">
+        <v>714</v>
+      </c>
+      <c r="R302" s="33" t="s">
         <v>713</v>
       </c>
-      <c r="Q302" s="33" t="s">
-        <v>715</v>
-      </c>
-      <c r="R302" s="33" t="s">
-        <v>714</v>
-      </c>
       <c r="S302" s="33" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="T302" s="31"/>
       <c r="U302" s="31"/>
@@ -19503,17 +19504,17 @@
       <c r="G303" s="31"/>
       <c r="H303" s="31"/>
       <c r="I303" s="33" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="J303" s="33" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="K303" s="31"/>
       <c r="L303" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M303" s="33" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="N303" s="31" t="s">
         <v>86</v>
@@ -19525,13 +19526,13 @@
         <v>242</v>
       </c>
       <c r="Q303" s="33" t="s">
+        <v>716</v>
+      </c>
+      <c r="R303" s="33" t="s">
         <v>717</v>
       </c>
-      <c r="R303" s="33" t="s">
-        <v>718</v>
-      </c>
       <c r="S303" s="33" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="T303" s="31"/>
       <c r="U303" s="31"/>
@@ -19553,17 +19554,17 @@
       <c r="G304" s="31"/>
       <c r="H304" s="31"/>
       <c r="I304" s="33" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="J304" s="33" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="K304" s="31"/>
       <c r="L304" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M304" s="33" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="N304" s="31" t="s">
         <v>86</v>
@@ -19575,13 +19576,13 @@
         <v>242</v>
       </c>
       <c r="Q304" s="33" t="s">
+        <v>716</v>
+      </c>
+      <c r="R304" s="33" t="s">
         <v>717</v>
       </c>
-      <c r="R304" s="33" t="s">
+      <c r="S304" s="33" t="s">
         <v>718</v>
-      </c>
-      <c r="S304" s="33" t="s">
-        <v>719</v>
       </c>
       <c r="T304" s="31"/>
       <c r="U304" s="31"/>
@@ -19603,17 +19604,17 @@
       <c r="G305" s="31"/>
       <c r="H305" s="31"/>
       <c r="I305" s="33" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="J305" s="33" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="K305" s="31"/>
       <c r="L305" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M305" s="33" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="N305" s="31" t="s">
         <v>85</v>
@@ -19625,10 +19626,10 @@
         <v>242</v>
       </c>
       <c r="Q305" s="33" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="R305" s="33" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="S305" s="31"/>
       <c r="T305" s="31"/>
@@ -19651,17 +19652,17 @@
       <c r="G306" s="31"/>
       <c r="H306" s="31"/>
       <c r="I306" s="33" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="J306" s="33" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="K306" s="31"/>
       <c r="L306" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M306" s="33" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="N306" s="31" t="s">
         <v>84</v>
@@ -19673,7 +19674,7 @@
         <v>242</v>
       </c>
       <c r="Q306" s="33" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="R306" s="31"/>
       <c r="S306" s="31"/>
@@ -19697,17 +19698,17 @@
       <c r="G307" s="31"/>
       <c r="H307" s="31"/>
       <c r="I307" s="33" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="J307" s="33" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="K307" s="31"/>
       <c r="L307" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M307" s="33" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="N307" s="31" t="s">
         <v>87</v>
@@ -19719,16 +19720,16 @@
         <v>242</v>
       </c>
       <c r="Q307" s="33" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="R307" s="33" t="s">
+        <v>723</v>
+      </c>
+      <c r="S307" s="33" t="s">
         <v>724</v>
       </c>
-      <c r="S307" s="33" t="s">
+      <c r="T307" s="33" t="s">
         <v>725</v>
-      </c>
-      <c r="T307" s="33" t="s">
-        <v>726</v>
       </c>
       <c r="U307" s="31"/>
       <c r="V307" s="31"/>
@@ -19749,10 +19750,10 @@
       <c r="G308" s="31"/>
       <c r="H308" s="31"/>
       <c r="I308" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="J308" s="33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="K308" s="31"/>
       <c r="L308" s="31" t="s">
@@ -19793,17 +19794,17 @@
       <c r="G309" s="31"/>
       <c r="H309" s="31"/>
       <c r="I309" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="J309" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="K309" s="31"/>
       <c r="L309" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M309" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="N309" s="31" t="s">
         <v>86</v>
@@ -19815,13 +19816,13 @@
         <v>242</v>
       </c>
       <c r="Q309" s="33" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="R309" s="33" t="s">
         <v>292</v>
       </c>
       <c r="S309" s="33" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="T309" s="31"/>
       <c r="U309" s="31"/>
@@ -19843,10 +19844,10 @@
       <c r="G310" s="31"/>
       <c r="H310" s="31"/>
       <c r="I310" s="33" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="J310" s="33" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="K310" s="31"/>
       <c r="L310" s="31" t="s">
@@ -19865,7 +19866,7 @@
         <v>242</v>
       </c>
       <c r="Q310" s="33" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="R310" s="33" t="s">
         <v>292</v>
@@ -19891,10 +19892,10 @@
       <c r="G311" s="31"/>
       <c r="H311" s="31"/>
       <c r="I311" s="33" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="J311" s="33" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="K311" s="31"/>
       <c r="L311" s="31" t="s">
@@ -19935,35 +19936,35 @@
       <c r="G312" s="31"/>
       <c r="H312" s="31"/>
       <c r="I312" s="33" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="J312" s="33" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="K312" s="31"/>
       <c r="L312" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M312" s="33" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="N312" s="31" t="s">
         <v>86</v>
       </c>
       <c r="O312" s="33" t="s">
+        <v>733</v>
+      </c>
+      <c r="P312" s="33" t="s">
         <v>734</v>
       </c>
-      <c r="P312" s="33" t="s">
+      <c r="Q312" s="33" t="s">
         <v>735</v>
       </c>
-      <c r="Q312" s="33" t="s">
+      <c r="R312" s="33" t="s">
         <v>736</v>
       </c>
-      <c r="R312" s="33" t="s">
-        <v>737</v>
-      </c>
       <c r="S312" s="33" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="T312" s="31"/>
       <c r="U312" s="31"/>
@@ -19985,23 +19986,23 @@
       <c r="G313" s="31"/>
       <c r="H313" s="31"/>
       <c r="I313" s="33" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="J313" s="33" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K313" s="31"/>
       <c r="L313" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M313" s="33" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="N313" s="31" t="s">
         <v>82</v>
       </c>
       <c r="O313" s="33" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="P313" s="31"/>
       <c r="Q313" s="31"/>
@@ -20027,17 +20028,17 @@
       <c r="G314" s="31"/>
       <c r="H314" s="31"/>
       <c r="I314" s="33" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="J314" s="33" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="K314" s="31"/>
       <c r="L314" s="31" t="s">
-        <v>489</v>
+        <v>787</v>
       </c>
       <c r="M314" s="33" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="N314" s="31"/>
       <c r="O314" s="31"/>
@@ -20057,44 +20058,44 @@
     </row>
     <row r="315" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I315" s="37" t="s">
+        <v>780</v>
+      </c>
+      <c r="J315" s="37" t="s">
+        <v>780</v>
+      </c>
+      <c r="L315" s="37" t="s">
         <v>781</v>
       </c>
-      <c r="J315" s="37" t="s">
+      <c r="M315" s="37" t="s">
         <v>781</v>
-      </c>
-      <c r="L315" s="37" t="s">
-        <v>782</v>
-      </c>
-      <c r="M315" s="37" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="316" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I316" s="39" t="s">
+        <v>782</v>
+      </c>
+      <c r="J316" s="39" t="s">
+        <v>782</v>
+      </c>
+      <c r="L316" s="37" t="s">
+        <v>781</v>
+      </c>
+      <c r="M316" s="37" t="s">
         <v>783</v>
-      </c>
-      <c r="J316" s="39" t="s">
-        <v>783</v>
-      </c>
-      <c r="L316" s="37" t="s">
-        <v>782</v>
-      </c>
-      <c r="M316" s="37" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="317" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I317" s="37" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="J317" s="37" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="L317" s="31" t="s">
         <v>207</v>
       </c>
       <c r="M317" s="33" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N317" s="31" t="s">
         <v>85</v>
@@ -20109,18 +20110,18 @@
         <v>274</v>
       </c>
       <c r="R317" s="33" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="318" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I318" s="37" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="J318" s="37" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="L318" s="37" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="M318" s="37" t="s">
         <v>317</v>
@@ -20134,9 +20135,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="R20" r:id="rId1" tooltip="Cyclopidae" display="https://en.wikipedia.org/wiki/Cyclopidae"/>
-    <hyperlink ref="R21" r:id="rId2" tooltip="Cyclopidae" display="https://en.wikipedia.org/wiki/Cyclopidae"/>
-    <hyperlink ref="R47" r:id="rId3" tooltip="Cyclopidae" display="https://en.wikipedia.org/wiki/Cyclopidae"/>
+    <hyperlink ref="R20" r:id="rId1" tooltip="Cyclopidae" display="https://en.wikipedia.org/wiki/Cyclopidae" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="R21" r:id="rId2" tooltip="Cyclopidae" display="https://en.wikipedia.org/wiki/Cyclopidae" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="R47" r:id="rId3" tooltip="Cyclopidae" display="https://en.wikipedia.org/wiki/Cyclopidae" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>